<commit_message>
- Updated wheelController open loop formula for Cozmo v3.2 - Added config file for cozmo v3.2
</commit_message>
<xml_diff>
--- a/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
+++ b/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="48000" windowHeight="19580" tabRatio="500" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="48000" windowHeight="19580" tabRatio="500" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Wheels" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Wheels v3 -MAX_WHEEL_SPEED=0.5" sheetId="6" r:id="rId6"/>
     <sheet name="Wheels v3 with low-D treads" sheetId="7" r:id="rId7"/>
     <sheet name="Lift v3" sheetId="8" r:id="rId8"/>
+    <sheet name="Wheels v3.2 wtreads" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
   <si>
     <t>Power</t>
   </si>
@@ -65,6 +66,9 @@
   </si>
   <si>
     <t>Some values faked for better zero crossing</t>
+  </si>
+  <si>
+    <t>MAX_WHEEL_SPEED = 0.75</t>
   </si>
 </sst>
 </file>
@@ -120,8 +124,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -165,7 +173,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -185,6 +193,8 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -204,6 +214,8 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,11 +465,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132863640"/>
-        <c:axId val="-2132860568"/>
+        <c:axId val="-2096456312"/>
+        <c:axId val="-2096453272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132863640"/>
+        <c:axId val="-2096456312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,12 +479,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132860568"/>
+        <c:crossAx val="-2096453272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132860568"/>
+        <c:axId val="-2096453272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,7 +495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132863640"/>
+        <c:crossAx val="-2096456312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -519,7 +531,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -552,7 +563,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -620,11 +630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135796872"/>
-        <c:axId val="-2135799688"/>
+        <c:axId val="-2089567976"/>
+        <c:axId val="-2089565160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135796872"/>
+        <c:axId val="-2089567976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -634,12 +644,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135799688"/>
+        <c:crossAx val="-2089565160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135799688"/>
+        <c:axId val="-2089565160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,14 +660,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135796872"/>
+        <c:crossAx val="-2089567976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -900,11 +909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135854680"/>
-        <c:axId val="-2135857640"/>
+        <c:axId val="-2089516312"/>
+        <c:axId val="-2089513352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135854680"/>
+        <c:axId val="-2089516312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -914,12 +923,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135857640"/>
+        <c:crossAx val="-2089513352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135857640"/>
+        <c:axId val="-2089513352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,7 +939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135854680"/>
+        <c:crossAx val="-2089516312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1083,11 +1092,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135885960"/>
-        <c:axId val="-2135888776"/>
+        <c:axId val="-2089485480"/>
+        <c:axId val="-2089482664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135885960"/>
+        <c:axId val="-2089485480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1097,12 +1106,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135888776"/>
+        <c:crossAx val="-2089482664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135888776"/>
+        <c:axId val="-2089482664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,7 +1122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135885960"/>
+        <c:crossAx val="-2089485480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1260,11 +1269,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135918728"/>
-        <c:axId val="-2135921544"/>
+        <c:axId val="-2089452712"/>
+        <c:axId val="-2089449896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135918728"/>
+        <c:axId val="-2089452712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,12 +1283,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135921544"/>
+        <c:crossAx val="-2089449896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135921544"/>
+        <c:axId val="-2089449896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,7 +1299,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135918728"/>
+        <c:crossAx val="-2089452712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1582,11 +1591,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111347624"/>
-        <c:axId val="-2111344808"/>
+        <c:axId val="-2089403048"/>
+        <c:axId val="-2089400232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111347624"/>
+        <c:axId val="-2089403048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,12 +1605,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111344808"/>
+        <c:crossAx val="-2089400232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111344808"/>
+        <c:axId val="-2089400232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1612,14 +1621,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111347624"/>
+        <c:crossAx val="-2089403048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1821,11 +1829,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111315912"/>
-        <c:axId val="-2111313032"/>
+        <c:axId val="-2093087784"/>
+        <c:axId val="-2093084824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111315912"/>
+        <c:axId val="-2093087784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1835,12 +1843,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111313032"/>
+        <c:crossAx val="-2093084824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111313032"/>
+        <c:axId val="-2093084824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1851,14 +1859,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111315912"/>
+        <c:crossAx val="-2093087784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1945,7 +1952,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="#,##0.000000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2055,11 +2061,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112417976"/>
-        <c:axId val="-2112420792"/>
+        <c:axId val="-2093049032"/>
+        <c:axId val="-2093046104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112417976"/>
+        <c:axId val="-2093049032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2069,12 +2075,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112420792"/>
+        <c:crossAx val="-2093046104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112420792"/>
+        <c:axId val="-2093046104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2085,14 +2091,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112417976"/>
+        <c:crossAx val="-2093049032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2365,11 +2370,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112453096"/>
-        <c:axId val="-2112455912"/>
+        <c:axId val="-2093013704"/>
+        <c:axId val="-2093010888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112453096"/>
+        <c:axId val="-2093013704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2379,12 +2384,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112455912"/>
+        <c:crossAx val="-2093010888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112455912"/>
+        <c:axId val="-2093010888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2395,7 +2400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112453096"/>
+        <c:crossAx val="-2093013704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2668,11 +2673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112487320"/>
-        <c:axId val="-2112490136"/>
+        <c:axId val="-2092979464"/>
+        <c:axId val="-2092976648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112487320"/>
+        <c:axId val="-2092979464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2682,12 +2687,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112490136"/>
+        <c:crossAx val="-2092976648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112490136"/>
+        <c:axId val="-2092976648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2698,7 +2703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112487320"/>
+        <c:crossAx val="-2092979464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2990,11 +2995,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112543544"/>
-        <c:axId val="-2112546360"/>
+        <c:axId val="-2093839800"/>
+        <c:axId val="-2093842616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112543544"/>
+        <c:axId val="-2093839800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3004,12 +3009,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112546360"/>
+        <c:crossAx val="-2093842616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112546360"/>
+        <c:axId val="-2093842616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3020,13 +3025,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112543544"/>
+        <c:crossAx val="-2093839800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3179,11 +3185,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111881432"/>
-        <c:axId val="-2111878616"/>
+        <c:axId val="-2093102904"/>
+        <c:axId val="-2093100008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111881432"/>
+        <c:axId val="-2093102904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3193,12 +3199,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111878616"/>
+        <c:crossAx val="-2093100008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111878616"/>
+        <c:axId val="-2093100008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3209,7 +3215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111881432"/>
+        <c:crossAx val="-2093102904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3417,11 +3423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112576184"/>
-        <c:axId val="-2112579000"/>
+        <c:axId val="-2093872440"/>
+        <c:axId val="-2093875256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112576184"/>
+        <c:axId val="-2093872440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3431,12 +3437,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112579000"/>
+        <c:crossAx val="-2093875256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112579000"/>
+        <c:axId val="-2093875256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3447,13 +3453,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112576184"/>
+        <c:crossAx val="-2093872440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3540,6 +3547,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="#,##0.00000000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3649,11 +3657,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112609624"/>
-        <c:axId val="-2112612504"/>
+        <c:axId val="-2093905848"/>
+        <c:axId val="-2093908728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112609624"/>
+        <c:axId val="-2093905848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3663,12 +3671,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112612504"/>
+        <c:crossAx val="-2093908728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112612504"/>
+        <c:axId val="-2093908728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3679,13 +3687,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112609624"/>
+        <c:crossAx val="-2093905848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3958,11 +3967,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112643608"/>
-        <c:axId val="-2112646424"/>
+        <c:axId val="-2093939864"/>
+        <c:axId val="-2093942680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112643608"/>
+        <c:axId val="-2093939864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3972,12 +3981,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112646424"/>
+        <c:crossAx val="-2093942680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112646424"/>
+        <c:axId val="-2093942680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3988,13 +3997,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112643608"/>
+        <c:crossAx val="-2093939864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4080,6 +4090,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -4261,11 +4272,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112677496"/>
-        <c:axId val="-2112680312"/>
+        <c:axId val="-2093973720"/>
+        <c:axId val="-2093976536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112677496"/>
+        <c:axId val="-2093973720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4275,12 +4286,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112680312"/>
+        <c:crossAx val="-2093976536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112680312"/>
+        <c:axId val="-2093976536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4291,13 +4302,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112677496"/>
+        <c:crossAx val="-2093973720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4542,11 +4554,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2107210824"/>
-        <c:axId val="-2107213784"/>
+        <c:axId val="-2038195240"/>
+        <c:axId val="-2038192280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2107210824"/>
+        <c:axId val="-2038195240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4556,12 +4568,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107213784"/>
+        <c:crossAx val="-2038192280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2107213784"/>
+        <c:axId val="-2038192280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4572,7 +4584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107210824"/>
+        <c:crossAx val="-2038195240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4752,11 +4764,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2110496056"/>
-        <c:axId val="-2110492888"/>
+        <c:axId val="-2038163576"/>
+        <c:axId val="-2038160760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2110496056"/>
+        <c:axId val="-2038163576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4766,12 +4778,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110492888"/>
+        <c:crossAx val="-2038160760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2110492888"/>
+        <c:axId val="-2038160760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4782,7 +4794,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110496056"/>
+        <c:crossAx val="-2038163576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4962,11 +4974,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2069936328"/>
-        <c:axId val="-2069938920"/>
+        <c:axId val="-2038130584"/>
+        <c:axId val="-2038127768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2069936328"/>
+        <c:axId val="-2038130584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4976,12 +4988,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2069938920"/>
+        <c:crossAx val="-2038127768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2069938920"/>
+        <c:axId val="-2038127768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4992,7 +5004,713 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2069936328"/>
+        <c:crossAx val="-2038130584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>122.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>172.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>193.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.286665786441329"/>
+                  <c:y val="0.0219323609139022"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>121.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2030587384"/>
+        <c:axId val="-2030584568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2030587384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030584568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2030584568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030587384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0579260404949381"/>
+                  <c:y val="0.028316961194183"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>122.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>172.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>193.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2030558136"/>
+        <c:axId val="-2030555352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2030558136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030555352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2030555352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030558136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0830721316085489"/>
+                  <c:y val="0.0417871707404652"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.00000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>121.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2030525800"/>
+        <c:axId val="-2030523016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2030525800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030523016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2030523016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030525800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5244,11 +5962,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133450600"/>
-        <c:axId val="-2133453560"/>
+        <c:axId val="-2091940088"/>
+        <c:axId val="-2091937128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133450600"/>
+        <c:axId val="-2091940088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5258,12 +5976,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133453560"/>
+        <c:crossAx val="-2091937128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133453560"/>
+        <c:axId val="-2091937128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5274,13 +5992,561 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133450600"/>
+        <c:crossAx val="-2091940088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.177273340832396"/>
+                  <c:y val="-0.0536174305573367"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$B$50:$B$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-193.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-172.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-148.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-122.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-95.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-70.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-41.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-26.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-11.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>122.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>172.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>193.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$50:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2030493016"/>
+        <c:axId val="-2030490200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2030493016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030490200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2030490200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030493016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0745858042342203"/>
+                  <c:y val="-0.0615458831534947"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$C$50:$C$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-192.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-170.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-145.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-121.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-95.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-70.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-39.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-25.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>121.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads'!$A$50:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2030456312"/>
+        <c:axId val="-2030453496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2030456312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030453496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2030453496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2030456312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5427,11 +6693,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133481224"/>
-        <c:axId val="-2133484040"/>
+        <c:axId val="-2092756504"/>
+        <c:axId val="-2092759320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133481224"/>
+        <c:axId val="-2092756504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5441,12 +6707,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133484040"/>
+        <c:crossAx val="-2092759320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133484040"/>
+        <c:axId val="-2092759320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5457,7 +6723,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133481224"/>
+        <c:crossAx val="-2092756504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5718,11 +6984,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133530776"/>
-        <c:axId val="-2133533736"/>
+        <c:axId val="-2092806088"/>
+        <c:axId val="-2092809048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133530776"/>
+        <c:axId val="-2092806088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5732,12 +6998,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133533736"/>
+        <c:crossAx val="-2092809048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133533736"/>
+        <c:axId val="-2092809048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5748,7 +7014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133530776"/>
+        <c:crossAx val="-2092806088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5907,11 +7173,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133561480"/>
-        <c:axId val="-2133564296"/>
+        <c:axId val="-2092836696"/>
+        <c:axId val="-2092839512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133561480"/>
+        <c:axId val="-2092836696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5921,12 +7187,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133564296"/>
+        <c:crossAx val="-2092839512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133564296"/>
+        <c:axId val="-2092839512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5937,7 +7203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133561480"/>
+        <c:crossAx val="-2092836696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6090,11 +7356,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133593976"/>
-        <c:axId val="-2133596792"/>
+        <c:axId val="-2092869192"/>
+        <c:axId val="-2092872008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133593976"/>
+        <c:axId val="-2092869192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6104,12 +7370,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133596792"/>
+        <c:crossAx val="-2092872008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133596792"/>
+        <c:axId val="-2092872008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6120,7 +7386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133593976"/>
+        <c:crossAx val="-2092869192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6195,7 +7461,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -6279,7 +7544,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -6347,11 +7611,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135726264"/>
-        <c:axId val="-2135729224"/>
+        <c:axId val="-2092920584"/>
+        <c:axId val="-2092923544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135726264"/>
+        <c:axId val="-2092920584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6361,12 +7625,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135729224"/>
+        <c:crossAx val="-2092923544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135729224"/>
+        <c:axId val="-2092923544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6377,14 +7641,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135726264"/>
+        <c:crossAx val="-2092920584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6414,7 +7677,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6520,11 +7782,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135763464"/>
-        <c:axId val="-2135766280"/>
+        <c:axId val="-2092951144"/>
+        <c:axId val="-2092953960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135763464"/>
+        <c:axId val="-2092951144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6534,12 +7796,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135766280"/>
+        <c:crossAx val="-2092953960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135766280"/>
+        <c:axId val="-2092953960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6550,14 +7812,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135763464"/>
+        <c:crossAx val="-2092951144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7432,6 +8693,171 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9913,7 +11339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
@@ -10035,6 +11461,379 @@
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="Y22" sqref="Y22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.3</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.35</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>122</v>
+      </c>
+      <c r="C8">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>148</v>
+      </c>
+      <c r="C9">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>172</v>
+      </c>
+      <c r="C10">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>193</v>
+      </c>
+      <c r="C11">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>-1</v>
+      </c>
+      <c r="B50">
+        <v>-193</v>
+      </c>
+      <c r="C50">
+        <v>-192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>-0.9</v>
+      </c>
+      <c r="B51">
+        <v>-172</v>
+      </c>
+      <c r="C51">
+        <v>-170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>-0.8</v>
+      </c>
+      <c r="B52">
+        <v>-148</v>
+      </c>
+      <c r="C52">
+        <v>-145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>-0.7</v>
+      </c>
+      <c r="B53">
+        <v>-122</v>
+      </c>
+      <c r="C53">
+        <v>-121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>-0.6</v>
+      </c>
+      <c r="B54">
+        <v>-95</v>
+      </c>
+      <c r="C54">
+        <v>-95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>-0.5</v>
+      </c>
+      <c r="B55">
+        <v>-70</v>
+      </c>
+      <c r="C55">
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>-0.4</v>
+      </c>
+      <c r="B56">
+        <v>-41</v>
+      </c>
+      <c r="C56">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>-0.35</v>
+      </c>
+      <c r="B57">
+        <v>-26</v>
+      </c>
+      <c r="C57">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>-0.3</v>
+      </c>
+      <c r="B58">
+        <v>-11</v>
+      </c>
+      <c r="C58">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>0.3</v>
+      </c>
+      <c r="B60">
+        <v>11</v>
+      </c>
+      <c r="C60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>0.35</v>
+      </c>
+      <c r="B61">
+        <v>26</v>
+      </c>
+      <c r="C61">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>0.4</v>
+      </c>
+      <c r="B62">
+        <v>41</v>
+      </c>
+      <c r="C62">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>0.5</v>
+      </c>
+      <c r="B63">
+        <v>70</v>
+      </c>
+      <c r="C63">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>0.6</v>
+      </c>
+      <c r="B64">
+        <v>95</v>
+      </c>
+      <c r="C64">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>0.7</v>
+      </c>
+      <c r="B65">
+        <v>122</v>
+      </c>
+      <c r="C65">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>0.8</v>
+      </c>
+      <c r="B66">
+        <v>148</v>
+      </c>
+      <c r="C66">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>0.9</v>
+      </c>
+      <c r="B67">
+        <v>172</v>
+      </c>
+      <c r="C67">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>193</v>
+      </c>
+      <c r="C68">
+        <v>192</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Retuned wheelController after encoder fix
</commit_message>
<xml_diff>
--- a/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
+++ b/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
@@ -465,11 +465,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2096456312"/>
-        <c:axId val="-2096453272"/>
+        <c:axId val="-2132186328"/>
+        <c:axId val="-2132183320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2096456312"/>
+        <c:axId val="-2132186328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,12 +479,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096453272"/>
+        <c:crossAx val="-2132183320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2096453272"/>
+        <c:axId val="-2132183320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096456312"/>
+        <c:crossAx val="-2132186328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -630,11 +630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089567976"/>
-        <c:axId val="-2089565160"/>
+        <c:axId val="-2131874424"/>
+        <c:axId val="-2131871608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089567976"/>
+        <c:axId val="-2131874424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,12 +644,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089565160"/>
+        <c:crossAx val="-2131871608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089565160"/>
+        <c:axId val="-2131871608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089567976"/>
+        <c:crossAx val="-2131874424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -909,11 +909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089516312"/>
-        <c:axId val="-2089513352"/>
+        <c:axId val="-2131823112"/>
+        <c:axId val="-2131820152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089516312"/>
+        <c:axId val="-2131823112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,12 +923,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089513352"/>
+        <c:crossAx val="-2131820152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089513352"/>
+        <c:axId val="-2131820152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,7 +939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089516312"/>
+        <c:crossAx val="-2131823112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1092,11 +1092,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089485480"/>
-        <c:axId val="-2089482664"/>
+        <c:axId val="-2131792280"/>
+        <c:axId val="-2131789464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089485480"/>
+        <c:axId val="-2131792280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,12 +1106,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089482664"/>
+        <c:crossAx val="-2131789464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089482664"/>
+        <c:axId val="-2131789464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089485480"/>
+        <c:crossAx val="-2131792280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1269,11 +1269,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089452712"/>
-        <c:axId val="-2089449896"/>
+        <c:axId val="-2132445432"/>
+        <c:axId val="-2132448248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089452712"/>
+        <c:axId val="-2132445432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,12 +1283,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089449896"/>
+        <c:crossAx val="-2132448248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089449896"/>
+        <c:axId val="-2132448248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1299,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089452712"/>
+        <c:crossAx val="-2132445432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1591,11 +1591,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089403048"/>
-        <c:axId val="-2089400232"/>
+        <c:axId val="-2132495064"/>
+        <c:axId val="-2132497880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089403048"/>
+        <c:axId val="-2132495064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1605,12 +1605,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089400232"/>
+        <c:crossAx val="-2132497880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089400232"/>
+        <c:axId val="-2132497880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089403048"/>
+        <c:crossAx val="-2132495064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1829,11 +1829,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093087784"/>
-        <c:axId val="-2093084824"/>
+        <c:axId val="-2135215384"/>
+        <c:axId val="-2135212424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093087784"/>
+        <c:axId val="-2135215384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,12 +1843,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093084824"/>
+        <c:crossAx val="-2135212424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093084824"/>
+        <c:axId val="-2135212424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1859,7 +1859,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093087784"/>
+        <c:crossAx val="-2135215384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2061,11 +2061,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093049032"/>
-        <c:axId val="-2093046104"/>
+        <c:axId val="-2132539128"/>
+        <c:axId val="-2132541944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093049032"/>
+        <c:axId val="-2132539128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2075,12 +2075,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093046104"/>
+        <c:crossAx val="-2132541944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093046104"/>
+        <c:axId val="-2132541944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2091,7 +2091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093049032"/>
+        <c:crossAx val="-2132539128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2370,11 +2370,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093013704"/>
-        <c:axId val="-2093010888"/>
+        <c:axId val="-2132573672"/>
+        <c:axId val="-2132576488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093013704"/>
+        <c:axId val="-2132573672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2384,12 +2384,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093010888"/>
+        <c:crossAx val="-2132576488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093010888"/>
+        <c:axId val="-2132576488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,7 +2400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093013704"/>
+        <c:crossAx val="-2132573672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2673,11 +2673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092979464"/>
-        <c:axId val="-2092976648"/>
+        <c:axId val="-2132607704"/>
+        <c:axId val="-2132610520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092979464"/>
+        <c:axId val="-2132607704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2687,12 +2687,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092976648"/>
+        <c:crossAx val="-2132610520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092976648"/>
+        <c:axId val="-2132610520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2703,7 +2703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092979464"/>
+        <c:crossAx val="-2132607704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2995,11 +2995,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093839800"/>
-        <c:axId val="-2093842616"/>
+        <c:axId val="-2132657432"/>
+        <c:axId val="-2132660248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093839800"/>
+        <c:axId val="-2132657432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3009,12 +3009,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093842616"/>
+        <c:crossAx val="-2132660248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093842616"/>
+        <c:axId val="-2132660248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,14 +3025,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093839800"/>
+        <c:crossAx val="-2132657432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3185,11 +3184,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093102904"/>
-        <c:axId val="-2093100008"/>
+        <c:axId val="-2134316504"/>
+        <c:axId val="-2134313608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093102904"/>
+        <c:axId val="-2134316504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3199,12 +3198,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093100008"/>
+        <c:crossAx val="-2134313608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093100008"/>
+        <c:axId val="-2134313608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3215,7 +3214,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093102904"/>
+        <c:crossAx val="-2134316504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3423,11 +3422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093872440"/>
-        <c:axId val="-2093875256"/>
+        <c:axId val="-2132690072"/>
+        <c:axId val="-2132692888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093872440"/>
+        <c:axId val="-2132690072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3437,12 +3436,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093875256"/>
+        <c:crossAx val="-2132692888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093875256"/>
+        <c:axId val="-2132692888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3453,14 +3452,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093872440"/>
+        <c:crossAx val="-2132690072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3547,7 +3545,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="#,##0.00000000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3657,11 +3654,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093905848"/>
-        <c:axId val="-2093908728"/>
+        <c:axId val="-2132723512"/>
+        <c:axId val="-2132726392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093905848"/>
+        <c:axId val="-2132723512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3671,12 +3668,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093908728"/>
+        <c:crossAx val="-2132726392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093908728"/>
+        <c:axId val="-2132726392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3687,14 +3684,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093905848"/>
+        <c:crossAx val="-2132723512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3967,11 +3963,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093939864"/>
-        <c:axId val="-2093942680"/>
+        <c:axId val="-2132757496"/>
+        <c:axId val="-2132760312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093939864"/>
+        <c:axId val="-2132757496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3981,12 +3977,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093942680"/>
+        <c:crossAx val="-2132760312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093942680"/>
+        <c:axId val="-2132760312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3997,14 +3993,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093939864"/>
+        <c:crossAx val="-2132757496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4090,7 +4085,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -4272,11 +4266,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093973720"/>
-        <c:axId val="-2093976536"/>
+        <c:axId val="-2132791384"/>
+        <c:axId val="-2132794200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093973720"/>
+        <c:axId val="-2132791384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4286,12 +4280,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093976536"/>
+        <c:crossAx val="-2132794200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093976536"/>
+        <c:axId val="-2132794200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4302,14 +4296,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093973720"/>
+        <c:crossAx val="-2132791384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4378,7 +4371,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -4474,7 +4466,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -4554,11 +4545,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2038195240"/>
-        <c:axId val="-2038192280"/>
+        <c:axId val="-2076819512"/>
+        <c:axId val="-2076816552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2038195240"/>
+        <c:axId val="-2076819512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4568,12 +4559,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2038192280"/>
+        <c:crossAx val="-2076816552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2038192280"/>
+        <c:axId val="-2076816552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4584,14 +4575,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2038195240"/>
+        <c:crossAx val="-2076819512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4636,7 +4626,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4764,11 +4753,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2038163576"/>
-        <c:axId val="-2038160760"/>
+        <c:axId val="-2076787848"/>
+        <c:axId val="-2076785032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2038163576"/>
+        <c:axId val="-2076787848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4778,12 +4767,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2038160760"/>
+        <c:crossAx val="-2076785032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2038160760"/>
+        <c:axId val="-2076785032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4794,14 +4783,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2038163576"/>
+        <c:crossAx val="-2076787848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4846,7 +4834,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4974,11 +4961,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2038130584"/>
-        <c:axId val="-2038127768"/>
+        <c:axId val="-2076754856"/>
+        <c:axId val="-2076752040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2038130584"/>
+        <c:axId val="-2076754856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4988,12 +4975,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2038127768"/>
+        <c:crossAx val="-2076752040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2038127768"/>
+        <c:axId val="-2076752040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5004,14 +4991,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2038130584"/>
+        <c:crossAx val="-2076754856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5108,31 +5094,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>11.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.0</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>122.0</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>148.0</c:v>
+                  <c:v>109.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>172.0</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>193.0</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5215,31 +5201,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>7.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.0</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121.0</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>145.0</c:v>
+                  <c:v>109.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>170.0</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>192.0</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5254,11 +5240,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2030587384"/>
-        <c:axId val="-2030584568"/>
+        <c:axId val="-2076706904"/>
+        <c:axId val="-2076704088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2030587384"/>
+        <c:axId val="-2076706904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5268,12 +5254,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030584568"/>
+        <c:crossAx val="-2076704088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2030584568"/>
+        <c:axId val="-2076704088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5284,7 +5270,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030587384"/>
+        <c:crossAx val="-2076706904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5392,31 +5378,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>11.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.0</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>122.0</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>148.0</c:v>
+                  <c:v>109.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>172.0</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>193.0</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5467,11 +5453,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2030558136"/>
-        <c:axId val="-2030555352"/>
+        <c:axId val="-2076674952"/>
+        <c:axId val="-2076672152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2030558136"/>
+        <c:axId val="-2076674952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5481,12 +5467,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030555352"/>
+        <c:crossAx val="-2076672152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2030555352"/>
+        <c:axId val="-2076672152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5497,7 +5483,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030558136"/>
+        <c:crossAx val="-2076674952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5591,8 +5577,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0830721316085489"/>
-                  <c:y val="0.0417871707404652"/>
+                  <c:x val="-0.123849409448819"/>
+                  <c:y val="0.0421526584421247"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.00000000000" sourceLinked="0"/>
@@ -5605,31 +5591,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>7.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.0</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121.0</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>145.0</c:v>
+                  <c:v>109.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>170.0</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>192.0</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5680,11 +5666,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2030525800"/>
-        <c:axId val="-2030523016"/>
+        <c:axId val="-2076641880"/>
+        <c:axId val="-2076639080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2030525800"/>
+        <c:axId val="-2076641880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5694,12 +5680,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030523016"/>
+        <c:crossAx val="-2076639080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2030523016"/>
+        <c:axId val="-2076639080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5710,7 +5696,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030525800"/>
+        <c:crossAx val="-2076641880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5962,11 +5948,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2091940088"/>
-        <c:axId val="-2091937128"/>
+        <c:axId val="-2132133736"/>
+        <c:axId val="-2132130776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2091940088"/>
+        <c:axId val="-2132133736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5976,12 +5962,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091937128"/>
+        <c:crossAx val="-2132130776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2091937128"/>
+        <c:axId val="-2132130776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5992,7 +5978,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091940088"/>
+        <c:crossAx val="-2132133736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6235,11 +6221,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2030493016"/>
-        <c:axId val="-2030490200"/>
+        <c:axId val="-2076608616"/>
+        <c:axId val="-2076605800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2030493016"/>
+        <c:axId val="-2076608616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6249,12 +6235,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030490200"/>
+        <c:crossAx val="-2076605800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2030490200"/>
+        <c:axId val="-2076605800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6265,7 +6251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030493016"/>
+        <c:crossAx val="-2076608616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6509,11 +6495,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2030456312"/>
-        <c:axId val="-2030453496"/>
+        <c:axId val="-2076576024"/>
+        <c:axId val="-2076573208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2030456312"/>
+        <c:axId val="-2076576024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6523,12 +6509,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030453496"/>
+        <c:crossAx val="-2076573208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2030453496"/>
+        <c:axId val="-2076573208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6539,7 +6525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030456312"/>
+        <c:crossAx val="-2076576024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6693,11 +6679,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092756504"/>
-        <c:axId val="-2092759320"/>
+        <c:axId val="-2132102856"/>
+        <c:axId val="-2132100040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092756504"/>
+        <c:axId val="-2132102856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6707,12 +6693,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092759320"/>
+        <c:crossAx val="-2132100040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092759320"/>
+        <c:axId val="-2132100040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6723,7 +6709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092756504"/>
+        <c:crossAx val="-2132102856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6984,11 +6970,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092806088"/>
-        <c:axId val="-2092809048"/>
+        <c:axId val="-2132053272"/>
+        <c:axId val="-2132050312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092806088"/>
+        <c:axId val="-2132053272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6998,12 +6984,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092809048"/>
+        <c:crossAx val="-2132050312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092809048"/>
+        <c:axId val="-2132050312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7014,7 +7000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092806088"/>
+        <c:crossAx val="-2132053272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7173,11 +7159,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092836696"/>
-        <c:axId val="-2092839512"/>
+        <c:axId val="-2132022568"/>
+        <c:axId val="-2132019752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092836696"/>
+        <c:axId val="-2132022568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7187,12 +7173,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092839512"/>
+        <c:crossAx val="-2132019752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092839512"/>
+        <c:axId val="-2132019752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7203,7 +7189,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092836696"/>
+        <c:crossAx val="-2132022568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7356,11 +7342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092869192"/>
-        <c:axId val="-2092872008"/>
+        <c:axId val="-2131990072"/>
+        <c:axId val="-2131987256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092869192"/>
+        <c:axId val="-2131990072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7370,12 +7356,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092872008"/>
+        <c:crossAx val="-2131987256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092872008"/>
+        <c:axId val="-2131987256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7386,7 +7372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092869192"/>
+        <c:crossAx val="-2131990072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7611,11 +7597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092920584"/>
-        <c:axId val="-2092923544"/>
+        <c:axId val="-2131938776"/>
+        <c:axId val="-2131935816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092920584"/>
+        <c:axId val="-2131938776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7625,12 +7611,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092923544"/>
+        <c:crossAx val="-2131935816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092923544"/>
+        <c:axId val="-2131935816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7641,7 +7627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092920584"/>
+        <c:crossAx val="-2131938776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7782,11 +7768,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092951144"/>
-        <c:axId val="-2092953960"/>
+        <c:axId val="-2131908184"/>
+        <c:axId val="-2131905368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092951144"/>
+        <c:axId val="-2131908184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7796,12 +7782,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092953960"/>
+        <c:crossAx val="-2131905368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092953960"/>
+        <c:axId val="-2131905368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7812,7 +7798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092951144"/>
+        <c:crossAx val="-2131908184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11479,7 +11465,7 @@
   <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="Y22" sqref="Y22"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11511,10 +11497,10 @@
         <v>0.3</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -11522,10 +11508,10 @@
         <v>0.35</v>
       </c>
       <c r="B4">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -11533,10 +11519,10 @@
         <v>0.4</v>
       </c>
       <c r="B5">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C5">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -11544,10 +11530,10 @@
         <v>0.5</v>
       </c>
       <c r="B6">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C6">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -11555,10 +11541,10 @@
         <v>0.6</v>
       </c>
       <c r="B7">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C7">
-        <v>95</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -11566,10 +11552,10 @@
         <v>0.7</v>
       </c>
       <c r="B8">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="C8">
-        <v>121</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -11577,10 +11563,10 @@
         <v>0.8</v>
       </c>
       <c r="B9">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="C9">
-        <v>145</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -11588,10 +11574,10 @@
         <v>0.9</v>
       </c>
       <c r="B10">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="C10">
-        <v>170</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -11599,10 +11585,10 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="C11">
-        <v>192</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:3">

</xml_diff>

<commit_message>
Lots of liftController changes: - power computation is purely based on PID position control. (No longer using current desired velocity) - SetAngularVelocity() is now effectively a controlled velocity as it uses SetDesiredHeight() - Removed all code related RECALIBRATE_AT_LIMITS since there's no more clutch. Went back to using CalibrationUpdate() on startup only. - Lift nodding may or may not work. Didn't test.
</commit_message>
<xml_diff>
--- a/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
+++ b/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="48000" windowHeight="19580" tabRatio="500" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="48000" windowHeight="19580" tabRatio="500" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Wheels" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Wheels v3 with low-D treads" sheetId="7" r:id="rId7"/>
     <sheet name="Lift v3" sheetId="8" r:id="rId8"/>
     <sheet name="Wheels v3.2 wtreads" sheetId="9" r:id="rId9"/>
+    <sheet name="Lift v3.2 (stronger motor)" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="14">
   <si>
     <t>Power</t>
   </si>
@@ -465,11 +466,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132186328"/>
-        <c:axId val="-2132183320"/>
+        <c:axId val="-2063563640"/>
+        <c:axId val="-2063566536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132186328"/>
+        <c:axId val="-2063563640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,12 +480,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132183320"/>
+        <c:crossAx val="-2063566536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132183320"/>
+        <c:axId val="-2063566536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +496,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132186328"/>
+        <c:crossAx val="-2063563640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -630,11 +631,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131874424"/>
-        <c:axId val="-2131871608"/>
+        <c:axId val="-2104401896"/>
+        <c:axId val="-2104399000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131874424"/>
+        <c:axId val="-2104401896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,12 +645,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131871608"/>
+        <c:crossAx val="-2104399000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131871608"/>
+        <c:axId val="-2104399000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +661,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131874424"/>
+        <c:crossAx val="-2104401896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -909,11 +910,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131823112"/>
-        <c:axId val="-2131820152"/>
+        <c:axId val="-2104350584"/>
+        <c:axId val="-2104347544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131823112"/>
+        <c:axId val="-2104350584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,12 +924,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131820152"/>
+        <c:crossAx val="-2104347544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131820152"/>
+        <c:axId val="-2104347544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,7 +940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131823112"/>
+        <c:crossAx val="-2104350584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1092,11 +1093,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131792280"/>
-        <c:axId val="-2131789464"/>
+        <c:axId val="-2104319752"/>
+        <c:axId val="-2104316856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131792280"/>
+        <c:axId val="-2104319752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,12 +1107,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131789464"/>
+        <c:crossAx val="-2104316856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131789464"/>
+        <c:axId val="-2104316856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1123,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131792280"/>
+        <c:crossAx val="-2104319752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1269,11 +1270,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132445432"/>
-        <c:axId val="-2132448248"/>
+        <c:axId val="-2104286984"/>
+        <c:axId val="-2104284088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132445432"/>
+        <c:axId val="-2104286984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,12 +1284,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132448248"/>
+        <c:crossAx val="-2104284088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132448248"/>
+        <c:axId val="-2104284088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132445432"/>
+        <c:crossAx val="-2104286984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1591,11 +1592,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132495064"/>
-        <c:axId val="-2132497880"/>
+        <c:axId val="-2104237352"/>
+        <c:axId val="-2104234456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132495064"/>
+        <c:axId val="-2104237352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1605,12 +1606,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132497880"/>
+        <c:crossAx val="-2104234456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132497880"/>
+        <c:axId val="-2104234456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1622,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132495064"/>
+        <c:crossAx val="-2104237352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1829,11 +1830,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135215384"/>
-        <c:axId val="-2135212424"/>
+        <c:axId val="-2098587736"/>
+        <c:axId val="-2098584776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135215384"/>
+        <c:axId val="-2098587736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,12 +1844,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135212424"/>
+        <c:crossAx val="-2098584776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135212424"/>
+        <c:axId val="-2098584776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1859,7 +1860,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135215384"/>
+        <c:crossAx val="-2098587736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2061,11 +2062,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132539128"/>
-        <c:axId val="-2132541944"/>
+        <c:axId val="-2098550440"/>
+        <c:axId val="-2098547512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132539128"/>
+        <c:axId val="-2098550440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2075,12 +2076,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132541944"/>
+        <c:crossAx val="-2098547512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132541944"/>
+        <c:axId val="-2098547512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2091,7 +2092,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132539128"/>
+        <c:crossAx val="-2098550440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2370,11 +2371,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132573672"/>
-        <c:axId val="-2132576488"/>
+        <c:axId val="-2098507864"/>
+        <c:axId val="-2098504968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132573672"/>
+        <c:axId val="-2098507864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2384,12 +2385,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132576488"/>
+        <c:crossAx val="-2098504968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132576488"/>
+        <c:axId val="-2098504968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,7 +2401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132573672"/>
+        <c:crossAx val="-2098507864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2673,11 +2674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132607704"/>
-        <c:axId val="-2132610520"/>
+        <c:axId val="-2098473640"/>
+        <c:axId val="-2098470744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132607704"/>
+        <c:axId val="-2098473640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2687,12 +2688,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132610520"/>
+        <c:crossAx val="-2098470744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132610520"/>
+        <c:axId val="-2098470744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2703,7 +2704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132607704"/>
+        <c:crossAx val="-2098473640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2995,11 +2996,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132657432"/>
-        <c:axId val="-2132660248"/>
+        <c:axId val="-2098417448"/>
+        <c:axId val="-2098414552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132657432"/>
+        <c:axId val="-2098417448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3009,12 +3010,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132660248"/>
+        <c:crossAx val="-2098414552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132660248"/>
+        <c:axId val="-2098414552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,7 +3026,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132657432"/>
+        <c:crossAx val="-2098417448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3184,11 +3185,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2134316504"/>
-        <c:axId val="-2134313608"/>
+        <c:axId val="-2062269784"/>
+        <c:axId val="-2062266968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2134316504"/>
+        <c:axId val="-2062269784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3198,12 +3199,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134313608"/>
+        <c:crossAx val="-2062266968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2134313608"/>
+        <c:axId val="-2062266968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3214,7 +3215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134316504"/>
+        <c:crossAx val="-2062269784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3422,11 +3423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132690072"/>
-        <c:axId val="-2132692888"/>
+        <c:axId val="-2098384856"/>
+        <c:axId val="-2098381928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132690072"/>
+        <c:axId val="-2098384856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3436,12 +3437,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132692888"/>
+        <c:crossAx val="-2098381928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132692888"/>
+        <c:axId val="-2098381928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3452,7 +3453,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132690072"/>
+        <c:crossAx val="-2098384856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3654,11 +3655,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132723512"/>
-        <c:axId val="-2132726392"/>
+        <c:axId val="-2098843240"/>
+        <c:axId val="-2098840280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132723512"/>
+        <c:axId val="-2098843240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3668,12 +3669,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132726392"/>
+        <c:crossAx val="-2098840280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132726392"/>
+        <c:axId val="-2098840280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3684,7 +3685,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132723512"/>
+        <c:crossAx val="-2098843240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3963,11 +3964,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132757496"/>
-        <c:axId val="-2132760312"/>
+        <c:axId val="-2098365176"/>
+        <c:axId val="-2098362392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132757496"/>
+        <c:axId val="-2098365176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3977,12 +3978,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132760312"/>
+        <c:crossAx val="-2098362392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132760312"/>
+        <c:axId val="-2098362392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3993,7 +3994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132757496"/>
+        <c:crossAx val="-2098365176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4266,11 +4267,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132791384"/>
-        <c:axId val="-2132794200"/>
+        <c:axId val="-2098951960"/>
+        <c:axId val="-2098949064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132791384"/>
+        <c:axId val="-2098951960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4280,12 +4281,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132794200"/>
+        <c:crossAx val="-2098949064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132794200"/>
+        <c:axId val="-2098949064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4296,7 +4297,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132791384"/>
+        <c:crossAx val="-2098951960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4371,6 +4372,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -4466,6 +4468,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -4545,11 +4548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076819512"/>
-        <c:axId val="-2076816552"/>
+        <c:axId val="-2098248664"/>
+        <c:axId val="-2098245624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076819512"/>
+        <c:axId val="-2098248664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4559,12 +4562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076816552"/>
+        <c:crossAx val="-2098245624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076816552"/>
+        <c:axId val="-2098245624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4575,13 +4578,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076819512"/>
+        <c:crossAx val="-2098248664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4626,6 +4630,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4753,11 +4758,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076787848"/>
-        <c:axId val="-2076785032"/>
+        <c:axId val="-2140135368"/>
+        <c:axId val="-2140132472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076787848"/>
+        <c:axId val="-2140135368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4767,12 +4772,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076785032"/>
+        <c:crossAx val="-2140132472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076785032"/>
+        <c:axId val="-2140132472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4783,13 +4788,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076787848"/>
+        <c:crossAx val="-2140135368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4834,6 +4840,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4961,11 +4968,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076754856"/>
-        <c:axId val="-2076752040"/>
+        <c:axId val="-2140102376"/>
+        <c:axId val="-2140099480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076754856"/>
+        <c:axId val="-2140102376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4975,12 +4982,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076752040"/>
+        <c:crossAx val="-2140099480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076752040"/>
+        <c:axId val="-2140099480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4991,13 +4998,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076754856"/>
+        <c:crossAx val="-2140102376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5240,11 +5248,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076706904"/>
-        <c:axId val="-2076704088"/>
+        <c:axId val="-2098219128"/>
+        <c:axId val="-2098971240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076706904"/>
+        <c:axId val="-2098219128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5254,12 +5262,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076704088"/>
+        <c:crossAx val="-2098971240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076704088"/>
+        <c:axId val="-2098971240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5270,7 +5278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076706904"/>
+        <c:crossAx val="-2098219128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5453,11 +5461,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076674952"/>
-        <c:axId val="-2076672152"/>
+        <c:axId val="-2099000376"/>
+        <c:axId val="-2099003192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076674952"/>
+        <c:axId val="-2099000376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5467,12 +5475,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076672152"/>
+        <c:crossAx val="-2099003192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076672152"/>
+        <c:axId val="-2099003192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5483,7 +5491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076674952"/>
+        <c:crossAx val="-2099000376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5666,11 +5674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076641880"/>
-        <c:axId val="-2076639080"/>
+        <c:axId val="-2099033448"/>
+        <c:axId val="-2099036264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076641880"/>
+        <c:axId val="-2099033448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5680,12 +5688,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076639080"/>
+        <c:crossAx val="-2099036264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076639080"/>
+        <c:axId val="-2099036264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5696,7 +5704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076641880"/>
+        <c:crossAx val="-2099033448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5948,11 +5956,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132133736"/>
-        <c:axId val="-2132130776"/>
+        <c:axId val="-2103469816"/>
+        <c:axId val="-2103605784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132133736"/>
+        <c:axId val="-2103469816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5962,12 +5970,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132130776"/>
+        <c:crossAx val="-2103605784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132130776"/>
+        <c:axId val="-2103605784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5978,7 +5986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132133736"/>
+        <c:crossAx val="-2103469816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6221,11 +6229,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076608616"/>
-        <c:axId val="-2076605800"/>
+        <c:axId val="-2099066696"/>
+        <c:axId val="-2099069512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076608616"/>
+        <c:axId val="-2099066696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6235,12 +6243,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076605800"/>
+        <c:crossAx val="-2099069512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076605800"/>
+        <c:axId val="-2099069512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6251,7 +6259,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076608616"/>
+        <c:crossAx val="-2099066696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6495,11 +6503,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076576024"/>
-        <c:axId val="-2076573208"/>
+        <c:axId val="-2099099304"/>
+        <c:axId val="-2099102120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076576024"/>
+        <c:axId val="-2099099304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6509,12 +6517,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076573208"/>
+        <c:crossAx val="-2099102120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076573208"/>
+        <c:axId val="-2099102120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6525,7 +6533,901 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076576024"/>
+        <c:crossAx val="-2099099304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0551179602549681"/>
+          <c:y val="0.0509259259259259"/>
+          <c:w val="0.764893888263967"/>
+          <c:h val="0.822469378827647"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UpSpeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DownSpeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2059326920"/>
+        <c:axId val="-2059329880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2059326920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2059329880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2059329880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2059326920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>UpPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0612814489349052"/>
+          <c:y val="0.18020202020202"/>
+          <c:w val="0.715281680950102"/>
+          <c:h val="0.713347013441502"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UpSpeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.121455315323154"/>
+                  <c:y val="0.0272778175455341"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$B$5:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$A$5:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2059356712"/>
+        <c:axId val="-2059359528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2059356712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2059359528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2059359528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2059356712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>DownPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0612814489349052"/>
+          <c:y val="0.18020202020202"/>
+          <c:w val="0.715281680950102"/>
+          <c:h val="0.713347013441502"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DownSpeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.121455315323154"/>
+                  <c:y val="0.0272778175455341"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$C$5:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lift v3.2 (stronger motor)'!$A$5:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2059388856"/>
+        <c:axId val="-2059391672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2059388856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2059391672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2059391672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2059388856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6679,11 +7581,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132102856"/>
-        <c:axId val="-2132100040"/>
+        <c:axId val="-2103758760"/>
+        <c:axId val="-2103755864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132102856"/>
+        <c:axId val="-2103758760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6693,12 +7595,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132100040"/>
+        <c:crossAx val="-2103755864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132100040"/>
+        <c:axId val="-2103755864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6709,7 +7611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132102856"/>
+        <c:crossAx val="-2103758760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6970,11 +7872,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132053272"/>
-        <c:axId val="-2132050312"/>
+        <c:axId val="-2103709176"/>
+        <c:axId val="-2103706136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132053272"/>
+        <c:axId val="-2103709176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6984,12 +7886,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132050312"/>
+        <c:crossAx val="-2103706136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132050312"/>
+        <c:axId val="-2103706136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7000,7 +7902,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132053272"/>
+        <c:crossAx val="-2103709176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7159,11 +8061,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132022568"/>
-        <c:axId val="-2132019752"/>
+        <c:axId val="-2103678472"/>
+        <c:axId val="-2103675576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132022568"/>
+        <c:axId val="-2103678472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7173,12 +8075,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132019752"/>
+        <c:crossAx val="-2103675576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132019752"/>
+        <c:axId val="-2103675576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7189,7 +8091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132022568"/>
+        <c:crossAx val="-2103678472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7342,11 +8244,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131990072"/>
-        <c:axId val="-2131987256"/>
+        <c:axId val="-2103645976"/>
+        <c:axId val="-2103784520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131990072"/>
+        <c:axId val="-2103645976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7356,12 +8258,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131987256"/>
+        <c:crossAx val="-2103784520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131987256"/>
+        <c:axId val="-2103784520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7372,7 +8274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131990072"/>
+        <c:crossAx val="-2103645976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7597,11 +8499,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131938776"/>
-        <c:axId val="-2131935816"/>
+        <c:axId val="-2104466248"/>
+        <c:axId val="-2104463208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131938776"/>
+        <c:axId val="-2104466248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7611,12 +8513,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131935816"/>
+        <c:crossAx val="-2104463208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131935816"/>
+        <c:axId val="-2104463208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7627,7 +8529,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131938776"/>
+        <c:crossAx val="-2104466248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7768,11 +8670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131908184"/>
-        <c:axId val="-2131905368"/>
+        <c:axId val="-2104435656"/>
+        <c:axId val="-2104432760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131908184"/>
+        <c:axId val="-2104435656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7782,12 +8684,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131905368"/>
+        <c:crossAx val="-2104432760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131905368"/>
+        <c:axId val="-2104432760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7798,7 +8700,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131908184"/>
+        <c:crossAx val="-2104435656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7876,6 +8778,107 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9379,6 +10382,244 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.25</v>
+      </c>
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.3</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.35</v>
+      </c>
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.4</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.45</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>0.6</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>0.65</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>0.7</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>0.75</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>0.8</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>0.85</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>0.9</v>
+      </c>
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>0.95000000000000095</v>
+      </c>
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
@@ -11464,7 +12705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Retuned wheelController since PWM cap was lifted on Espressif robot
</commit_message>
<xml_diff>
--- a/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
+++ b/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="48000" windowHeight="19580" tabRatio="500" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="1220" yWindow="0" windowWidth="48000" windowHeight="19580" tabRatio="500" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Wheels" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Lift v3" sheetId="8" r:id="rId8"/>
     <sheet name="Wheels v3.2 wtreads" sheetId="9" r:id="rId9"/>
     <sheet name="Lift v3.2 (stronger motor)" sheetId="10" r:id="rId10"/>
+    <sheet name="Wheels v3.2 wtreads (Espressif)" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="14">
   <si>
     <t>Power</t>
   </si>
@@ -125,8 +126,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -174,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -196,6 +199,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -217,6 +221,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,11 +471,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2063563640"/>
-        <c:axId val="-2063566536"/>
+        <c:axId val="-2142624216"/>
+        <c:axId val="-2142621352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2063563640"/>
+        <c:axId val="-2142624216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,12 +485,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063566536"/>
+        <c:crossAx val="-2142621352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2063566536"/>
+        <c:axId val="-2142621352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +501,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063563640"/>
+        <c:crossAx val="-2142624216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -631,11 +636,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104401896"/>
-        <c:axId val="-2104399000"/>
+        <c:axId val="-2139411608"/>
+        <c:axId val="-2139408792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104401896"/>
+        <c:axId val="-2139411608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,12 +650,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104399000"/>
+        <c:crossAx val="-2139408792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104399000"/>
+        <c:axId val="-2139408792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +666,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104401896"/>
+        <c:crossAx val="-2139411608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -910,11 +915,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104350584"/>
-        <c:axId val="-2104347544"/>
+        <c:axId val="-2142564888"/>
+        <c:axId val="-2142561928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104350584"/>
+        <c:axId val="-2142564888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,12 +929,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104347544"/>
+        <c:crossAx val="-2142561928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104347544"/>
+        <c:axId val="-2142561928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,7 +945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104350584"/>
+        <c:crossAx val="-2142564888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1093,11 +1098,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104319752"/>
-        <c:axId val="-2104316856"/>
+        <c:axId val="-2142534056"/>
+        <c:axId val="-2142531240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104319752"/>
+        <c:axId val="-2142534056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,12 +1112,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104316856"/>
+        <c:crossAx val="-2142531240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104316856"/>
+        <c:axId val="-2142531240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1123,7 +1128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104319752"/>
+        <c:crossAx val="-2142534056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1270,11 +1275,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104286984"/>
-        <c:axId val="-2104284088"/>
+        <c:axId val="-2142501288"/>
+        <c:axId val="-2142498472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104286984"/>
+        <c:axId val="-2142501288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,12 +1289,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104284088"/>
+        <c:crossAx val="-2142498472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104284088"/>
+        <c:axId val="-2142498472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104286984"/>
+        <c:crossAx val="-2142501288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1592,11 +1597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104237352"/>
-        <c:axId val="-2104234456"/>
+        <c:axId val="-2145779736"/>
+        <c:axId val="-2145776840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104237352"/>
+        <c:axId val="-2145779736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,12 +1611,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104234456"/>
+        <c:crossAx val="-2145776840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104234456"/>
+        <c:axId val="-2145776840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1622,7 +1627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104237352"/>
+        <c:crossAx val="-2145779736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1830,11 +1835,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098587736"/>
-        <c:axId val="-2098584776"/>
+        <c:axId val="-2145743976"/>
+        <c:axId val="-2145741016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098587736"/>
+        <c:axId val="-2145743976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,12 +1849,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098584776"/>
+        <c:crossAx val="-2145741016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098584776"/>
+        <c:axId val="-2145741016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1860,7 +1865,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098587736"/>
+        <c:crossAx val="-2145743976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2062,11 +2067,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098550440"/>
-        <c:axId val="-2098547512"/>
+        <c:axId val="-2141359064"/>
+        <c:axId val="-2141356264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098550440"/>
+        <c:axId val="-2141359064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2076,12 +2081,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098547512"/>
+        <c:crossAx val="-2141356264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098547512"/>
+        <c:axId val="-2141356264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2092,7 +2097,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098550440"/>
+        <c:crossAx val="-2141359064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2371,11 +2376,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098507864"/>
-        <c:axId val="-2098504968"/>
+        <c:axId val="2047416632"/>
+        <c:axId val="2047420168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098507864"/>
+        <c:axId val="2047416632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2385,12 +2390,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098504968"/>
+        <c:crossAx val="2047420168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098504968"/>
+        <c:axId val="2047420168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,7 +2406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098507864"/>
+        <c:crossAx val="2047416632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2674,11 +2679,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098473640"/>
-        <c:axId val="-2098470744"/>
+        <c:axId val="2047459896"/>
+        <c:axId val="2047462792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098473640"/>
+        <c:axId val="2047459896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2688,12 +2693,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098470744"/>
+        <c:crossAx val="2047462792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098470744"/>
+        <c:axId val="2047462792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2704,7 +2709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098473640"/>
+        <c:crossAx val="2047459896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2996,11 +3001,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098417448"/>
-        <c:axId val="-2098414552"/>
+        <c:axId val="2047515832"/>
+        <c:axId val="2047518648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098417448"/>
+        <c:axId val="2047515832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3010,12 +3015,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098414552"/>
+        <c:crossAx val="2047518648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098414552"/>
+        <c:axId val="2047518648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3026,7 +3031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098417448"/>
+        <c:crossAx val="2047515832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3185,11 +3190,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062269784"/>
-        <c:axId val="-2062266968"/>
+        <c:axId val="-2139517496"/>
+        <c:axId val="-2139514680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062269784"/>
+        <c:axId val="-2139517496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3199,12 +3204,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062266968"/>
+        <c:crossAx val="-2139514680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2062266968"/>
+        <c:axId val="-2139514680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3215,7 +3220,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062269784"/>
+        <c:crossAx val="-2139517496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3423,11 +3428,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098384856"/>
-        <c:axId val="-2098381928"/>
+        <c:axId val="2047548472"/>
+        <c:axId val="2047551272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098384856"/>
+        <c:axId val="2047548472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3437,12 +3442,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098381928"/>
+        <c:crossAx val="2047551272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098381928"/>
+        <c:axId val="2047551272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3453,7 +3458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098384856"/>
+        <c:crossAx val="2047548472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3655,11 +3660,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098843240"/>
-        <c:axId val="-2098840280"/>
+        <c:axId val="2047581896"/>
+        <c:axId val="2047584776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098843240"/>
+        <c:axId val="2047581896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3669,12 +3674,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098840280"/>
+        <c:crossAx val="2047584776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098840280"/>
+        <c:axId val="2047584776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3685,7 +3690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098843240"/>
+        <c:crossAx val="2047581896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3964,11 +3969,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098365176"/>
-        <c:axId val="-2098362392"/>
+        <c:axId val="-2145711992"/>
+        <c:axId val="-2145709096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098365176"/>
+        <c:axId val="-2145711992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3978,12 +3983,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098362392"/>
+        <c:crossAx val="-2145709096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098362392"/>
+        <c:axId val="-2145709096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3994,7 +3999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098365176"/>
+        <c:crossAx val="-2145711992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4267,11 +4272,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098951960"/>
-        <c:axId val="-2098949064"/>
+        <c:axId val="-2145677976"/>
+        <c:axId val="-2145675080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098951960"/>
+        <c:axId val="-2145677976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4281,12 +4286,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098949064"/>
+        <c:crossAx val="-2145675080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098949064"/>
+        <c:axId val="-2145675080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4297,7 +4302,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098951960"/>
+        <c:crossAx val="-2145677976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4372,7 +4377,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -4468,7 +4472,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -4548,11 +4551,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098248664"/>
-        <c:axId val="-2098245624"/>
+        <c:axId val="-2145590296"/>
+        <c:axId val="-2145587256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098248664"/>
+        <c:axId val="-2145590296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4562,12 +4565,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098245624"/>
+        <c:crossAx val="-2145587256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098245624"/>
+        <c:axId val="-2145587256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4578,14 +4581,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098248664"/>
+        <c:crossAx val="-2145590296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4630,7 +4632,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4758,11 +4759,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140135368"/>
-        <c:axId val="-2140132472"/>
+        <c:axId val="-2145558632"/>
+        <c:axId val="-2145555736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140135368"/>
+        <c:axId val="-2145558632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4772,12 +4773,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140132472"/>
+        <c:crossAx val="-2145555736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140132472"/>
+        <c:axId val="-2145555736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4788,14 +4789,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140135368"/>
+        <c:crossAx val="-2145558632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4840,7 +4840,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4968,11 +4967,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140102376"/>
-        <c:axId val="-2140099480"/>
+        <c:axId val="-2145522552"/>
+        <c:axId val="-2145519656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140102376"/>
+        <c:axId val="-2145522552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4982,12 +4981,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140099480"/>
+        <c:crossAx val="-2145519656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140099480"/>
+        <c:axId val="-2145519656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4998,14 +4997,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140102376"/>
+        <c:crossAx val="-2145522552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5248,11 +5246,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098219128"/>
-        <c:axId val="-2098971240"/>
+        <c:axId val="-2145474600"/>
+        <c:axId val="-2145471704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098219128"/>
+        <c:axId val="-2145474600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5262,12 +5260,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098971240"/>
+        <c:crossAx val="-2145471704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098971240"/>
+        <c:axId val="-2145471704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5278,7 +5276,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098219128"/>
+        <c:crossAx val="-2145474600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5461,11 +5459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2099000376"/>
-        <c:axId val="-2099003192"/>
+        <c:axId val="2049107896"/>
+        <c:axId val="2049110824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2099000376"/>
+        <c:axId val="2049107896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5475,12 +5473,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099003192"/>
+        <c:crossAx val="2049110824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2099003192"/>
+        <c:axId val="2049110824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5491,7 +5489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099000376"/>
+        <c:crossAx val="2049107896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5674,11 +5672,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2099033448"/>
-        <c:axId val="-2099036264"/>
+        <c:axId val="2049146584"/>
+        <c:axId val="2049149512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2099033448"/>
+        <c:axId val="2049146584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5688,12 +5686,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099036264"/>
+        <c:crossAx val="2049149512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2099036264"/>
+        <c:axId val="2049149512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5704,7 +5702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099033448"/>
+        <c:crossAx val="2049146584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5956,11 +5954,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103469816"/>
-        <c:axId val="-2103605784"/>
+        <c:axId val="-2141396200"/>
+        <c:axId val="-2141393240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103469816"/>
+        <c:axId val="-2141396200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5970,12 +5968,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103605784"/>
+        <c:crossAx val="-2141393240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103605784"/>
+        <c:axId val="-2141393240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5986,7 +5984,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103469816"/>
+        <c:crossAx val="-2141396200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6229,11 +6227,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2099066696"/>
-        <c:axId val="-2099069512"/>
+        <c:axId val="2049180632"/>
+        <c:axId val="2049183528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2099066696"/>
+        <c:axId val="2049180632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6243,12 +6241,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099069512"/>
+        <c:crossAx val="2049183528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2099069512"/>
+        <c:axId val="2049183528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6259,7 +6257,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099066696"/>
+        <c:crossAx val="2049180632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6503,11 +6501,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2099099304"/>
-        <c:axId val="-2099102120"/>
+        <c:axId val="2049057832"/>
+        <c:axId val="2049214392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2099099304"/>
+        <c:axId val="2049057832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6517,12 +6515,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099102120"/>
+        <c:crossAx val="2049214392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2099102120"/>
+        <c:axId val="2049214392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6533,7 +6531,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099099304"/>
+        <c:crossAx val="2049057832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6893,11 +6891,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059326920"/>
-        <c:axId val="-2059329880"/>
+        <c:axId val="2049025816"/>
+        <c:axId val="2049022856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059326920"/>
+        <c:axId val="2049025816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6907,12 +6905,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059329880"/>
+        <c:crossAx val="2049022856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059329880"/>
+        <c:axId val="2049022856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6923,7 +6921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059326920"/>
+        <c:crossAx val="2049025816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7145,11 +7143,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059356712"/>
-        <c:axId val="-2059359528"/>
+        <c:axId val="2048994168"/>
+        <c:axId val="2048991352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059356712"/>
+        <c:axId val="2048994168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7159,12 +7157,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059359528"/>
+        <c:crossAx val="2048991352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059359528"/>
+        <c:axId val="2048991352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7175,7 +7173,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059356712"/>
+        <c:crossAx val="2048994168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7397,11 +7395,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059388856"/>
-        <c:axId val="-2059391672"/>
+        <c:axId val="2048960200"/>
+        <c:axId val="2048957384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059388856"/>
+        <c:axId val="2048960200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7411,12 +7409,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059391672"/>
+        <c:crossAx val="2048957384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059391672"/>
+        <c:axId val="2048957384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7427,7 +7425,1261 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059388856"/>
+        <c:crossAx val="2048960200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>202.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>228.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>255.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.286665786441329"/>
+                  <c:y val="0.0219323609139022"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>134.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>191.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2066434104"/>
+        <c:axId val="-2066436920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2066434104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2066436920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2066436920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2066434104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0579260404949381"/>
+                  <c:y val="0.028316961194183"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>202.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>228.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>255.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2066463896"/>
+        <c:axId val="-2066466712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2066463896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2066466712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2066466712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2066463896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.123849409448819"/>
+                  <c:y val="0.0421526584421247"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.00000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>134.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>191.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2029375160"/>
+        <c:axId val="2029378088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2029375160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2029378088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2029378088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2029375160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.177273340832396"/>
+                  <c:y val="-0.0536174305573367"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$B$50:$B$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-255.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-228.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-202.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-173.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-145.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-115.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-86.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-48.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>202.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>228.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>255.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$50:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2066497752"/>
+        <c:axId val="-2066500568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2066497752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2066500568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2066500568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2066497752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0745858042342203"/>
+                  <c:y val="-0.0615458831534947"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$C$50:$C$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-240.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-220.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-191.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-162.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-134.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-105.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-72.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-42.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>105.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>134.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>191.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>240.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v3.2 wtreads (Espressif)'!$A$50:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2069681224"/>
+        <c:axId val="-2069684040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2069681224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2069684040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2069684040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2069681224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7581,11 +8833,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103758760"/>
-        <c:axId val="-2103755864"/>
+        <c:axId val="-2140653240"/>
+        <c:axId val="-2140649048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103758760"/>
+        <c:axId val="-2140653240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7595,12 +8847,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103755864"/>
+        <c:crossAx val="-2140649048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103755864"/>
+        <c:axId val="-2140649048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7611,7 +8863,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103758760"/>
+        <c:crossAx val="-2140653240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7872,11 +9124,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103709176"/>
-        <c:axId val="-2103706136"/>
+        <c:axId val="-2140567944"/>
+        <c:axId val="-2140564984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103709176"/>
+        <c:axId val="-2140567944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7886,12 +9138,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103706136"/>
+        <c:crossAx val="-2140564984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103706136"/>
+        <c:axId val="-2140564984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7902,7 +9154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103709176"/>
+        <c:crossAx val="-2140567944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8061,11 +9313,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103678472"/>
-        <c:axId val="-2103675576"/>
+        <c:axId val="-2140537240"/>
+        <c:axId val="-2140534424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103678472"/>
+        <c:axId val="-2140537240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8075,12 +9327,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103675576"/>
+        <c:crossAx val="-2140534424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103675576"/>
+        <c:axId val="-2140534424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8091,7 +9343,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103678472"/>
+        <c:crossAx val="-2140537240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8244,11 +9496,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103645976"/>
-        <c:axId val="-2103784520"/>
+        <c:axId val="-2140504744"/>
+        <c:axId val="-2140501928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103645976"/>
+        <c:axId val="-2140504744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8258,12 +9510,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103784520"/>
+        <c:crossAx val="-2140501928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103784520"/>
+        <c:axId val="-2140501928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8274,7 +9526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103645976"/>
+        <c:crossAx val="-2140504744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8499,11 +9751,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104466248"/>
-        <c:axId val="-2104463208"/>
+        <c:axId val="-2139476056"/>
+        <c:axId val="-2139473096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104466248"/>
+        <c:axId val="-2139476056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8513,12 +9765,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104463208"/>
+        <c:crossAx val="-2139473096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104463208"/>
+        <c:axId val="-2139473096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8529,7 +9781,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104466248"/>
+        <c:crossAx val="-2139476056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8670,11 +9922,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104435656"/>
-        <c:axId val="-2104432760"/>
+        <c:axId val="-2139445016"/>
+        <c:axId val="-2139442200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104435656"/>
+        <c:axId val="-2139445016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8684,12 +9936,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104432760"/>
+        <c:crossAx val="-2139442200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104432760"/>
+        <c:axId val="-2139442200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8700,7 +9952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104435656"/>
+        <c:crossAx val="-2139445016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8879,6 +10131,171 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10386,7 +11803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -10607,6 +12024,369 @@
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="M74" sqref="M74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>86</v>
+      </c>
+      <c r="C5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>115</v>
+      </c>
+      <c r="C6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>145</v>
+      </c>
+      <c r="C7">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>173</v>
+      </c>
+      <c r="C8">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>202</v>
+      </c>
+      <c r="C9">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>228</v>
+      </c>
+      <c r="C10">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>255</v>
+      </c>
+      <c r="C11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>-1</v>
+      </c>
+      <c r="B50">
+        <v>-255</v>
+      </c>
+      <c r="C50">
+        <v>-240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>-0.9</v>
+      </c>
+      <c r="B51">
+        <v>-228</v>
+      </c>
+      <c r="C51">
+        <v>-220</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>-0.8</v>
+      </c>
+      <c r="B52">
+        <v>-202</v>
+      </c>
+      <c r="C52">
+        <v>-191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>-0.7</v>
+      </c>
+      <c r="B53">
+        <v>-173</v>
+      </c>
+      <c r="C53">
+        <v>-162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>-0.6</v>
+      </c>
+      <c r="B54">
+        <v>-145</v>
+      </c>
+      <c r="C54">
+        <v>-134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>-0.5</v>
+      </c>
+      <c r="B55">
+        <v>-115</v>
+      </c>
+      <c r="C55">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>-0.4</v>
+      </c>
+      <c r="B56">
+        <v>-86</v>
+      </c>
+      <c r="C56">
+        <v>-72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>-0.3</v>
+      </c>
+      <c r="B57">
+        <v>-48</v>
+      </c>
+      <c r="C57">
+        <v>-42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>-0.2</v>
+      </c>
+      <c r="B58">
+        <v>-10</v>
+      </c>
+      <c r="C58">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>0.2</v>
+      </c>
+      <c r="B60">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>0.3</v>
+      </c>
+      <c r="B61">
+        <v>48</v>
+      </c>
+      <c r="C61">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>0.4</v>
+      </c>
+      <c r="B62">
+        <v>86</v>
+      </c>
+      <c r="C62">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>0.5</v>
+      </c>
+      <c r="B63">
+        <v>115</v>
+      </c>
+      <c r="C63">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>0.6</v>
+      </c>
+      <c r="B64">
+        <v>145</v>
+      </c>
+      <c r="C64">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>0.7</v>
+      </c>
+      <c r="B65">
+        <v>173</v>
+      </c>
+      <c r="C65">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>0.8</v>
+      </c>
+      <c r="B66">
+        <v>202</v>
+      </c>
+      <c r="C66">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>0.9</v>
+      </c>
+      <c r="B67">
+        <v>228</v>
+      </c>
+      <c r="C67">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>255</v>
+      </c>
+      <c r="C68">
+        <v>240</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Retuned wheelController since move to cozmo 4. Didn't really change much. Increased fov of simulated camera in cozmoBot.
</commit_message>
<xml_diff>
--- a/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
+++ b/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="0" windowWidth="48000" windowHeight="19580" tabRatio="500" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="10620" yWindow="0" windowWidth="35160" windowHeight="19580" tabRatio="500" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Wheels" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Wheels v3.2 wtreads" sheetId="9" r:id="rId9"/>
     <sheet name="Lift v3.2 (stronger motor)" sheetId="10" r:id="rId10"/>
     <sheet name="Wheels v3.2 wtreads (Espressif)" sheetId="11" r:id="rId11"/>
+    <sheet name="Wheels v4" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
   <si>
     <t>Power</t>
   </si>
@@ -471,11 +472,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2142624216"/>
-        <c:axId val="-2142621352"/>
+        <c:axId val="-2029548328"/>
+        <c:axId val="-2029545448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2142624216"/>
+        <c:axId val="-2029548328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -485,12 +486,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142621352"/>
+        <c:crossAx val="-2029545448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2142621352"/>
+        <c:axId val="-2029545448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,7 +502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142624216"/>
+        <c:crossAx val="-2029548328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -636,11 +637,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2139411608"/>
-        <c:axId val="-2139408792"/>
+        <c:axId val="-2029435624"/>
+        <c:axId val="-2029432840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2139411608"/>
+        <c:axId val="-2029435624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,12 +651,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139408792"/>
+        <c:crossAx val="-2029432840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2139408792"/>
+        <c:axId val="-2029432840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139411608"/>
+        <c:crossAx val="-2029435624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -915,11 +916,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2142564888"/>
-        <c:axId val="-2142561928"/>
+        <c:axId val="-2029377720"/>
+        <c:axId val="-2029374792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2142564888"/>
+        <c:axId val="-2029377720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,12 +930,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142561928"/>
+        <c:crossAx val="-2029374792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2142561928"/>
+        <c:axId val="-2029374792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,7 +946,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142564888"/>
+        <c:crossAx val="-2029377720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1098,11 +1099,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2142534056"/>
-        <c:axId val="-2142531240"/>
+        <c:axId val="-2029346888"/>
+        <c:axId val="-2029344104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2142534056"/>
+        <c:axId val="-2029346888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1112,12 +1113,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142531240"/>
+        <c:crossAx val="-2029344104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2142531240"/>
+        <c:axId val="-2029344104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142534056"/>
+        <c:crossAx val="-2029346888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1275,11 +1276,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2142501288"/>
-        <c:axId val="-2142498472"/>
+        <c:axId val="-2029314120"/>
+        <c:axId val="-2029311336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2142501288"/>
+        <c:axId val="-2029314120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1289,12 +1290,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142498472"/>
+        <c:crossAx val="-2029311336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2142498472"/>
+        <c:axId val="-2029311336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1305,7 +1306,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142501288"/>
+        <c:crossAx val="-2029314120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1597,11 +1598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145779736"/>
-        <c:axId val="-2145776840"/>
+        <c:axId val="-2029264488"/>
+        <c:axId val="-2029261704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145779736"/>
+        <c:axId val="-2029264488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1611,12 +1612,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145776840"/>
+        <c:crossAx val="-2029261704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145776840"/>
+        <c:axId val="-2029261704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1627,7 +1628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145779736"/>
+        <c:crossAx val="-2029264488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1835,11 +1836,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145743976"/>
-        <c:axId val="-2145741016"/>
+        <c:axId val="-2094026600"/>
+        <c:axId val="-2094023752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145743976"/>
+        <c:axId val="-2094026600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,12 +1850,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145741016"/>
+        <c:crossAx val="-2094023752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145741016"/>
+        <c:axId val="-2094023752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1865,7 +1866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145743976"/>
+        <c:crossAx val="-2094026600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2067,11 +2068,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2141359064"/>
-        <c:axId val="-2141356264"/>
+        <c:axId val="-2028319144"/>
+        <c:axId val="-2028316376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2141359064"/>
+        <c:axId val="-2028319144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,12 +2082,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141356264"/>
+        <c:crossAx val="-2028316376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2141356264"/>
+        <c:axId val="-2028316376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2097,7 +2098,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141359064"/>
+        <c:crossAx val="-2028319144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2376,11 +2377,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2047416632"/>
-        <c:axId val="2047420168"/>
+        <c:axId val="-2028283912"/>
+        <c:axId val="-2028281128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2047416632"/>
+        <c:axId val="-2028283912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2390,12 +2391,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047420168"/>
+        <c:crossAx val="-2028281128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2047420168"/>
+        <c:axId val="-2028281128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2406,7 +2407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047416632"/>
+        <c:crossAx val="-2028283912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2679,11 +2680,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2047459896"/>
-        <c:axId val="2047462792"/>
+        <c:axId val="-2028249688"/>
+        <c:axId val="-2028246904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2047459896"/>
+        <c:axId val="-2028249688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2693,12 +2694,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047462792"/>
+        <c:crossAx val="-2028246904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2047462792"/>
+        <c:axId val="-2028246904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2709,7 +2710,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047459896"/>
+        <c:crossAx val="-2028249688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3001,11 +3002,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2047515832"/>
-        <c:axId val="2047518648"/>
+        <c:axId val="-2028193528"/>
+        <c:axId val="-2028190744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2047515832"/>
+        <c:axId val="-2028193528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3015,12 +3016,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047518648"/>
+        <c:crossAx val="-2028190744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2047518648"/>
+        <c:axId val="-2028190744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3031,7 +3032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047515832"/>
+        <c:crossAx val="-2028193528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3190,11 +3191,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2139517496"/>
-        <c:axId val="-2139514680"/>
+        <c:axId val="-2090764696"/>
+        <c:axId val="-2090767448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2139517496"/>
+        <c:axId val="-2090764696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3204,12 +3205,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139514680"/>
+        <c:crossAx val="-2090767448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2139514680"/>
+        <c:axId val="-2090767448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3220,7 +3221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139517496"/>
+        <c:crossAx val="-2090764696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3428,11 +3429,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2047548472"/>
-        <c:axId val="2047551272"/>
+        <c:axId val="-2028160872"/>
+        <c:axId val="-2028158120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2047548472"/>
+        <c:axId val="-2028160872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3442,12 +3443,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047551272"/>
+        <c:crossAx val="-2028158120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2047551272"/>
+        <c:axId val="-2028158120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3458,7 +3459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047548472"/>
+        <c:crossAx val="-2028160872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3660,11 +3661,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2047581896"/>
-        <c:axId val="2047584776"/>
+        <c:axId val="-2028127464"/>
+        <c:axId val="-2028124616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2047581896"/>
+        <c:axId val="-2028127464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3674,12 +3675,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047584776"/>
+        <c:crossAx val="-2028124616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2047584776"/>
+        <c:axId val="-2028124616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3690,7 +3691,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047581896"/>
+        <c:crossAx val="-2028127464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3969,11 +3970,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145711992"/>
-        <c:axId val="-2145709096"/>
+        <c:axId val="-2028093464"/>
+        <c:axId val="-2028090680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145711992"/>
+        <c:axId val="-2028093464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3983,12 +3984,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145709096"/>
+        <c:crossAx val="-2028090680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145709096"/>
+        <c:axId val="-2028090680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3999,7 +4000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145711992"/>
+        <c:crossAx val="-2028093464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4272,11 +4273,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145677976"/>
-        <c:axId val="-2145675080"/>
+        <c:axId val="-2028059608"/>
+        <c:axId val="-2028056824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145677976"/>
+        <c:axId val="-2028059608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4286,12 +4287,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145675080"/>
+        <c:crossAx val="-2028056824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145675080"/>
+        <c:axId val="-2028056824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4302,7 +4303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145677976"/>
+        <c:crossAx val="-2028059608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4551,11 +4552,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145590296"/>
-        <c:axId val="-2145587256"/>
+        <c:axId val="-2090811112"/>
+        <c:axId val="-2090814008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145590296"/>
+        <c:axId val="-2090811112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4565,12 +4566,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145587256"/>
+        <c:crossAx val="-2090814008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145587256"/>
+        <c:axId val="-2090814008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4581,7 +4582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145590296"/>
+        <c:crossAx val="-2090811112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4759,11 +4760,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145558632"/>
-        <c:axId val="-2145555736"/>
+        <c:axId val="-2090842808"/>
+        <c:axId val="-2090845560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145558632"/>
+        <c:axId val="-2090842808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4773,12 +4774,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145555736"/>
+        <c:crossAx val="-2090845560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145555736"/>
+        <c:axId val="-2090845560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4789,7 +4790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145558632"/>
+        <c:crossAx val="-2090842808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4967,11 +4968,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145522552"/>
-        <c:axId val="-2145519656"/>
+        <c:axId val="-2027530920"/>
+        <c:axId val="-2027528136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145522552"/>
+        <c:axId val="-2027530920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4981,12 +4982,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145519656"/>
+        <c:crossAx val="-2027528136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145519656"/>
+        <c:axId val="-2027528136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4997,7 +4998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145522552"/>
+        <c:crossAx val="-2027530920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5246,11 +5247,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145474600"/>
-        <c:axId val="-2145471704"/>
+        <c:axId val="-2027482744"/>
+        <c:axId val="-2027479960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145474600"/>
+        <c:axId val="-2027482744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5260,12 +5261,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145471704"/>
+        <c:crossAx val="-2027479960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145471704"/>
+        <c:axId val="-2027479960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5276,14 +5277,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145474600"/>
+        <c:crossAx val="-2027482744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5459,11 +5459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2049107896"/>
-        <c:axId val="2049110824"/>
+        <c:axId val="-2027450328"/>
+        <c:axId val="-2027447576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2049107896"/>
+        <c:axId val="-2027450328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5473,12 +5473,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049110824"/>
+        <c:crossAx val="-2027447576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2049110824"/>
+        <c:axId val="-2027447576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5489,14 +5489,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049107896"/>
+        <c:crossAx val="-2027450328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5672,11 +5671,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2049146584"/>
-        <c:axId val="2049149512"/>
+        <c:axId val="-2028023000"/>
+        <c:axId val="-2028020248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2049146584"/>
+        <c:axId val="-2028023000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5686,12 +5685,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049149512"/>
+        <c:crossAx val="-2028020248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2049149512"/>
+        <c:axId val="-2028020248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5702,14 +5701,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049146584"/>
+        <c:crossAx val="-2028023000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5954,11 +5952,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2141396200"/>
-        <c:axId val="-2141393240"/>
+        <c:axId val="-2029497224"/>
+        <c:axId val="-2029494296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2141396200"/>
+        <c:axId val="-2029497224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5968,12 +5966,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141393240"/>
+        <c:crossAx val="-2029494296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2141393240"/>
+        <c:axId val="-2029494296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5984,7 +5982,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141396200"/>
+        <c:crossAx val="-2029497224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6227,11 +6225,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2049180632"/>
-        <c:axId val="2049183528"/>
+        <c:axId val="-2027990152"/>
+        <c:axId val="-2027987368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2049180632"/>
+        <c:axId val="-2027990152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6241,12 +6239,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049183528"/>
+        <c:crossAx val="-2027987368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2049183528"/>
+        <c:axId val="-2027987368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6257,14 +6255,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049180632"/>
+        <c:crossAx val="-2027990152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6501,11 +6498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2049057832"/>
-        <c:axId val="2049214392"/>
+        <c:axId val="-2028599560"/>
+        <c:axId val="-2028602312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2049057832"/>
+        <c:axId val="-2028599560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6515,12 +6512,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049214392"/>
+        <c:crossAx val="-2028602312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2049214392"/>
+        <c:axId val="-2028602312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6531,14 +6528,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049057832"/>
+        <c:crossAx val="-2028599560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6891,11 +6887,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2049025816"/>
-        <c:axId val="2049022856"/>
+        <c:axId val="-2028659528"/>
+        <c:axId val="-2028662424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2049025816"/>
+        <c:axId val="-2028659528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6905,12 +6901,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049022856"/>
+        <c:crossAx val="-2028662424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2049022856"/>
+        <c:axId val="-2028662424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6921,7 +6917,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049025816"/>
+        <c:crossAx val="-2028659528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7143,11 +7139,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2048994168"/>
-        <c:axId val="2048991352"/>
+        <c:axId val="-2028691176"/>
+        <c:axId val="-2028693928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2048994168"/>
+        <c:axId val="-2028691176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7157,12 +7153,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048991352"/>
+        <c:crossAx val="-2028693928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2048991352"/>
+        <c:axId val="-2028693928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7173,7 +7169,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048994168"/>
+        <c:crossAx val="-2028691176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7395,11 +7391,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2048960200"/>
-        <c:axId val="2048957384"/>
+        <c:axId val="-2028724856"/>
+        <c:axId val="-2028727608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2048960200"/>
+        <c:axId val="-2028724856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7409,12 +7405,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048957384"/>
+        <c:crossAx val="-2028727608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2048957384"/>
+        <c:axId val="-2028727608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7425,7 +7421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048960200"/>
+        <c:crossAx val="-2028724856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7675,11 +7671,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2066434104"/>
-        <c:axId val="-2066436920"/>
+        <c:axId val="-2094674696"/>
+        <c:axId val="-2094677448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2066434104"/>
+        <c:axId val="-2094674696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7689,12 +7685,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066436920"/>
+        <c:crossAx val="-2094677448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2066436920"/>
+        <c:axId val="-2094677448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7705,7 +7701,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066434104"/>
+        <c:crossAx val="-2094674696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7888,11 +7884,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2066463896"/>
-        <c:axId val="-2066466712"/>
+        <c:axId val="-2094710952"/>
+        <c:axId val="-2094713704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2066463896"/>
+        <c:axId val="-2094710952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7902,12 +7898,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066466712"/>
+        <c:crossAx val="-2094713704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2066466712"/>
+        <c:axId val="-2094713704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7918,7 +7914,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066463896"/>
+        <c:crossAx val="-2094710952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8101,11 +8097,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2029375160"/>
-        <c:axId val="2029378088"/>
+        <c:axId val="-2094744120"/>
+        <c:axId val="-2094746872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2029375160"/>
+        <c:axId val="-2094744120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8115,12 +8111,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2029378088"/>
+        <c:crossAx val="-2094746872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2029378088"/>
+        <c:axId val="-2094746872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8131,7 +8127,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2029375160"/>
+        <c:crossAx val="-2094744120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8375,11 +8371,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2066497752"/>
-        <c:axId val="-2066500568"/>
+        <c:axId val="-2094777656"/>
+        <c:axId val="-2094780408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2066497752"/>
+        <c:axId val="-2094777656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8389,12 +8385,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066500568"/>
+        <c:crossAx val="-2094780408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2066500568"/>
+        <c:axId val="-2094780408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8405,7 +8401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066497752"/>
+        <c:crossAx val="-2094777656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8649,11 +8645,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2069681224"/>
-        <c:axId val="-2069684040"/>
+        <c:axId val="-2029252872"/>
+        <c:axId val="-2029245944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2069681224"/>
+        <c:axId val="-2029252872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8663,12 +8659,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2069684040"/>
+        <c:crossAx val="-2029245944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2069684040"/>
+        <c:axId val="-2029245944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8679,7 +8675,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2069681224"/>
+        <c:crossAx val="-2029252872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8833,11 +8829,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140653240"/>
-        <c:axId val="-2140649048"/>
+        <c:axId val="-2029466600"/>
+        <c:axId val="-2029463816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140653240"/>
+        <c:axId val="-2029466600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8847,12 +8843,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140649048"/>
+        <c:crossAx val="-2029463816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140649048"/>
+        <c:axId val="-2029463816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8863,13 +8859,719 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140653240"/>
+        <c:crossAx val="-2029466600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v4'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v4'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v4'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>171.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>225.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>247.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v4'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.286665786441329"/>
+                  <c:y val="0.0219323609139022"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v4'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v4'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>202.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>228.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>249.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2019832808"/>
+        <c:axId val="-2019830024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2019832808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2019830024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2019830024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2019832808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v4'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0579260404949381"/>
+                  <c:y val="0.028316961194183"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v4'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>171.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>225.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>247.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v4'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2023513688"/>
+        <c:axId val="-2023516456"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2023513688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2023516456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2023516456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2023513688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v4'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.123849409448819"/>
+                  <c:y val="0.0421526584421247"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.00000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v4'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>202.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>228.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>249.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v4'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2021800552"/>
+        <c:axId val="-2021844376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2021800552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2021844376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2021844376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2021800552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9124,11 +9826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140567944"/>
-        <c:axId val="-2140564984"/>
+        <c:axId val="-2028415944"/>
+        <c:axId val="-2028413016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140567944"/>
+        <c:axId val="-2028415944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9138,12 +9840,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140564984"/>
+        <c:crossAx val="-2028413016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140564984"/>
+        <c:axId val="-2028413016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9154,7 +9856,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140567944"/>
+        <c:crossAx val="-2028415944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9313,11 +10015,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140537240"/>
-        <c:axId val="-2140534424"/>
+        <c:axId val="-2028385240"/>
+        <c:axId val="-2028382456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140537240"/>
+        <c:axId val="-2028385240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9327,12 +10029,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140534424"/>
+        <c:crossAx val="-2028382456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140534424"/>
+        <c:axId val="-2028382456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9343,7 +10045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140537240"/>
+        <c:crossAx val="-2028385240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9496,11 +10198,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140504744"/>
-        <c:axId val="-2140501928"/>
+        <c:axId val="-2028352744"/>
+        <c:axId val="-2028349960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140504744"/>
+        <c:axId val="-2028352744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9510,12 +10212,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140501928"/>
+        <c:crossAx val="-2028349960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140501928"/>
+        <c:axId val="-2028349960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9526,7 +10228,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140504744"/>
+        <c:crossAx val="-2028352744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9751,11 +10453,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2139476056"/>
-        <c:axId val="-2139473096"/>
+        <c:axId val="-2094069016"/>
+        <c:axId val="-2094066088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2139476056"/>
+        <c:axId val="-2094069016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9765,12 +10467,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139473096"/>
+        <c:crossAx val="-2094066088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2139473096"/>
+        <c:axId val="-2094066088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9781,7 +10483,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139476056"/>
+        <c:crossAx val="-2094069016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9922,11 +10624,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2139445016"/>
-        <c:axId val="-2139442200"/>
+        <c:axId val="-2094038424"/>
+        <c:axId val="-2094035640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2139445016"/>
+        <c:axId val="-2094038424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9936,12 +10638,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139442200"/>
+        <c:crossAx val="-2094035640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2139442200"/>
+        <c:axId val="-2094035640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9952,7 +10654,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139445016"/>
+        <c:crossAx val="-2094038424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10296,6 +10998,107 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11804,7 +12607,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12041,7 +12844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="M74" sqref="M74"/>
     </sheetView>
   </sheetViews>
@@ -12386,6 +13189,149 @@
       </c>
       <c r="C68">
         <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>52</v>
+      </c>
+      <c r="C4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>88</v>
+      </c>
+      <c r="C5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>118</v>
+      </c>
+      <c r="C6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>146</v>
+      </c>
+      <c r="C7">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>171</v>
+      </c>
+      <c r="C8">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>225</v>
+      </c>
+      <c r="C10">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>247</v>
+      </c>
+      <c r="C11">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Added cozmoConfig_v4.1.h with new camera calibration * Updated wheelController and liftController for 4.1 robot
</commit_message>
<xml_diff>
--- a/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
+++ b/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="0" windowWidth="35160" windowHeight="19580" tabRatio="500" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="39640" yWindow="0" windowWidth="35160" windowHeight="19580" tabRatio="500" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Wheels" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Lift v3.2 (stronger motor)" sheetId="10" r:id="rId10"/>
     <sheet name="Wheels v3.2 wtreads (Espressif)" sheetId="11" r:id="rId11"/>
     <sheet name="Wheels v4" sheetId="12" r:id="rId12"/>
+    <sheet name="Wheels v4.1" sheetId="13" r:id="rId13"/>
+    <sheet name="Lift v4.1" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="14">
   <si>
     <t>Power</t>
   </si>
@@ -472,11 +474,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2029548328"/>
-        <c:axId val="-2029545448"/>
+        <c:axId val="-2126498824"/>
+        <c:axId val="-2064074696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2029548328"/>
+        <c:axId val="-2126498824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,12 +488,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029545448"/>
+        <c:crossAx val="-2064074696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2029545448"/>
+        <c:axId val="-2064074696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -502,7 +504,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029548328"/>
+        <c:crossAx val="-2126498824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -637,11 +639,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2029435624"/>
-        <c:axId val="-2029432840"/>
+        <c:axId val="-2063157864"/>
+        <c:axId val="2048445528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2029435624"/>
+        <c:axId val="-2063157864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,12 +653,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029432840"/>
+        <c:crossAx val="2048445528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2029432840"/>
+        <c:axId val="2048445528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,7 +669,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029435624"/>
+        <c:crossAx val="-2063157864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -916,11 +918,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2029377720"/>
-        <c:axId val="-2029374792"/>
+        <c:axId val="-2062785400"/>
+        <c:axId val="-2063200680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2029377720"/>
+        <c:axId val="-2062785400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,12 +932,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029374792"/>
+        <c:crossAx val="-2063200680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2029374792"/>
+        <c:axId val="-2063200680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +948,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029377720"/>
+        <c:crossAx val="-2062785400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1099,11 +1101,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2029346888"/>
-        <c:axId val="-2029344104"/>
+        <c:axId val="-2063212408"/>
+        <c:axId val="-2063210184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2029346888"/>
+        <c:axId val="-2063212408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,12 +1115,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029344104"/>
+        <c:crossAx val="-2063210184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2029344104"/>
+        <c:axId val="-2063210184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,7 +1131,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029346888"/>
+        <c:crossAx val="-2063212408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1276,11 +1278,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2029314120"/>
-        <c:axId val="-2029311336"/>
+        <c:axId val="-2123290504"/>
+        <c:axId val="-2123287608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2029314120"/>
+        <c:axId val="-2123290504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,12 +1292,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029311336"/>
+        <c:crossAx val="-2123287608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2029311336"/>
+        <c:axId val="-2123287608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,7 +1308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029314120"/>
+        <c:crossAx val="-2123290504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1598,11 +1600,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2029264488"/>
-        <c:axId val="-2029261704"/>
+        <c:axId val="-2122466040"/>
+        <c:axId val="-2122488136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2029264488"/>
+        <c:axId val="-2122466040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1612,12 +1614,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029261704"/>
+        <c:crossAx val="-2122488136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2029261704"/>
+        <c:axId val="-2122488136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1628,7 +1630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029264488"/>
+        <c:crossAx val="-2122466040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1836,11 +1838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094026600"/>
-        <c:axId val="-2094023752"/>
+        <c:axId val="-2059792344"/>
+        <c:axId val="-2059789384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094026600"/>
+        <c:axId val="-2059792344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1850,12 +1852,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094023752"/>
+        <c:crossAx val="-2059789384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094023752"/>
+        <c:axId val="-2059789384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1866,7 +1868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094026600"/>
+        <c:crossAx val="-2059792344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2068,11 +2070,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028319144"/>
-        <c:axId val="-2028316376"/>
+        <c:axId val="-2059995096"/>
+        <c:axId val="-2059996920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028319144"/>
+        <c:axId val="-2059995096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2082,12 +2084,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028316376"/>
+        <c:crossAx val="-2059996920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028316376"/>
+        <c:axId val="-2059996920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,7 +2100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028319144"/>
+        <c:crossAx val="-2059995096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2377,11 +2379,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028283912"/>
-        <c:axId val="-2028281128"/>
+        <c:axId val="2047556136"/>
+        <c:axId val="2047559032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028283912"/>
+        <c:axId val="2047556136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,12 +2393,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028281128"/>
+        <c:crossAx val="2047559032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028281128"/>
+        <c:axId val="2047559032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2407,7 +2409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028283912"/>
+        <c:crossAx val="2047556136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2680,11 +2682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028249688"/>
-        <c:axId val="-2028246904"/>
+        <c:axId val="-2059827224"/>
+        <c:axId val="-2059824328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028249688"/>
+        <c:axId val="-2059827224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2694,12 +2696,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028246904"/>
+        <c:crossAx val="-2059824328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028246904"/>
+        <c:axId val="-2059824328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2710,7 +2712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028249688"/>
+        <c:crossAx val="-2059827224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3002,11 +3004,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028193528"/>
-        <c:axId val="-2028190744"/>
+        <c:axId val="-2071545752"/>
+        <c:axId val="-2063735064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028193528"/>
+        <c:axId val="-2071545752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3016,12 +3018,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028190744"/>
+        <c:crossAx val="-2063735064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028190744"/>
+        <c:axId val="-2063735064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3032,7 +3034,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028193528"/>
+        <c:crossAx val="-2071545752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3191,11 +3193,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090764696"/>
-        <c:axId val="-2090767448"/>
+        <c:axId val="-2064170312"/>
+        <c:axId val="-2063639048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2090764696"/>
+        <c:axId val="-2064170312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3205,12 +3207,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090767448"/>
+        <c:crossAx val="-2063639048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2090767448"/>
+        <c:axId val="-2063639048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3221,7 +3223,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090764696"/>
+        <c:crossAx val="-2064170312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3429,11 +3431,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028160872"/>
-        <c:axId val="-2028158120"/>
+        <c:axId val="-2063744568"/>
+        <c:axId val="-2063741640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028160872"/>
+        <c:axId val="-2063744568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3443,12 +3445,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028158120"/>
+        <c:crossAx val="-2063741640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028158120"/>
+        <c:axId val="-2063741640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3459,7 +3461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028160872"/>
+        <c:crossAx val="-2063744568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3661,11 +3663,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028127464"/>
-        <c:axId val="-2028124616"/>
+        <c:axId val="-2064144392"/>
+        <c:axId val="-2126456392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028127464"/>
+        <c:axId val="-2064144392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3675,12 +3677,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028124616"/>
+        <c:crossAx val="-2126456392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028124616"/>
+        <c:axId val="-2126456392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3691,7 +3693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028127464"/>
+        <c:crossAx val="-2064144392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3970,11 +3972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028093464"/>
-        <c:axId val="-2028090680"/>
+        <c:axId val="-2063932184"/>
+        <c:axId val="-2063929288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028093464"/>
+        <c:axId val="-2063932184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3984,12 +3986,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028090680"/>
+        <c:crossAx val="-2063929288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028090680"/>
+        <c:axId val="-2063929288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4000,7 +4002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028093464"/>
+        <c:crossAx val="-2063932184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4273,11 +4275,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028059608"/>
-        <c:axId val="-2028056824"/>
+        <c:axId val="-2064385400"/>
+        <c:axId val="-2064314344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028059608"/>
+        <c:axId val="-2064385400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4287,12 +4289,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028056824"/>
+        <c:crossAx val="-2064314344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028056824"/>
+        <c:axId val="-2064314344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4303,7 +4305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028059608"/>
+        <c:crossAx val="-2064385400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4552,11 +4554,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090811112"/>
-        <c:axId val="-2090814008"/>
+        <c:axId val="-2064193656"/>
+        <c:axId val="-2064190920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2090811112"/>
+        <c:axId val="-2064193656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4566,12 +4568,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090814008"/>
+        <c:crossAx val="-2064190920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2090814008"/>
+        <c:axId val="-2064190920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4582,7 +4584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090811112"/>
+        <c:crossAx val="-2064193656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4760,11 +4762,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090842808"/>
-        <c:axId val="-2090845560"/>
+        <c:axId val="-2064160392"/>
+        <c:axId val="-2064157496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2090842808"/>
+        <c:axId val="-2064160392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4774,12 +4776,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090845560"/>
+        <c:crossAx val="-2064157496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2090845560"/>
+        <c:axId val="-2064157496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4790,7 +4792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090842808"/>
+        <c:crossAx val="-2064160392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4968,11 +4970,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2027530920"/>
-        <c:axId val="-2027528136"/>
+        <c:axId val="-2071392264"/>
+        <c:axId val="-2071389368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2027530920"/>
+        <c:axId val="-2071392264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4982,12 +4984,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027528136"/>
+        <c:crossAx val="-2071389368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2027528136"/>
+        <c:axId val="-2071389368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4998,7 +5000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027530920"/>
+        <c:crossAx val="-2071392264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5247,11 +5249,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2027482744"/>
-        <c:axId val="-2027479960"/>
+        <c:axId val="-2062008792"/>
+        <c:axId val="-2062110792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2027482744"/>
+        <c:axId val="-2062008792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5261,12 +5263,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027479960"/>
+        <c:crossAx val="-2062110792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2027479960"/>
+        <c:axId val="-2062110792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5277,7 +5279,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027482744"/>
+        <c:crossAx val="-2062008792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5459,11 +5461,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2027450328"/>
-        <c:axId val="-2027447576"/>
+        <c:axId val="2123533960"/>
+        <c:axId val="2123724296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2027450328"/>
+        <c:axId val="2123533960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5473,12 +5475,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027447576"/>
+        <c:crossAx val="2123724296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2027447576"/>
+        <c:axId val="2123724296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5489,7 +5491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027450328"/>
+        <c:crossAx val="2123533960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5671,11 +5673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028023000"/>
-        <c:axId val="-2028020248"/>
+        <c:axId val="-2061757560"/>
+        <c:axId val="-2123098376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028023000"/>
+        <c:axId val="-2061757560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5685,12 +5687,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028020248"/>
+        <c:crossAx val="-2123098376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028020248"/>
+        <c:axId val="-2123098376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5701,7 +5703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028023000"/>
+        <c:crossAx val="-2061757560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5952,11 +5954,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2029497224"/>
-        <c:axId val="-2029494296"/>
+        <c:axId val="-2071975464"/>
+        <c:axId val="-2071972424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2029497224"/>
+        <c:axId val="-2071975464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5966,12 +5968,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029494296"/>
+        <c:crossAx val="-2071972424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2029494296"/>
+        <c:axId val="-2071972424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5982,7 +5984,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029497224"/>
+        <c:crossAx val="-2071975464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6225,11 +6227,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2027990152"/>
-        <c:axId val="-2027987368"/>
+        <c:axId val="-2062669512"/>
+        <c:axId val="-2063293016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2027990152"/>
+        <c:axId val="-2062669512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6239,12 +6241,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027987368"/>
+        <c:crossAx val="-2063293016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2027987368"/>
+        <c:axId val="-2063293016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6255,7 +6257,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027990152"/>
+        <c:crossAx val="-2062669512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6498,11 +6500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028599560"/>
-        <c:axId val="-2028602312"/>
+        <c:axId val="-2067736616"/>
+        <c:axId val="-2067767400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028599560"/>
+        <c:axId val="-2067736616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6512,12 +6514,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028602312"/>
+        <c:crossAx val="-2067767400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028602312"/>
+        <c:axId val="-2067767400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6528,7 +6530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028599560"/>
+        <c:crossAx val="-2067736616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6887,11 +6889,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028659528"/>
-        <c:axId val="-2028662424"/>
+        <c:axId val="-2062609144"/>
+        <c:axId val="-2062773752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028659528"/>
+        <c:axId val="-2062609144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6901,12 +6903,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028662424"/>
+        <c:crossAx val="-2062773752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028662424"/>
+        <c:axId val="-2062773752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6917,7 +6919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028659528"/>
+        <c:crossAx val="-2062609144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7139,11 +7141,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028691176"/>
-        <c:axId val="-2028693928"/>
+        <c:axId val="-2067621688"/>
+        <c:axId val="2048435288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028691176"/>
+        <c:axId val="-2067621688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7153,12 +7155,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028693928"/>
+        <c:crossAx val="2048435288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028693928"/>
+        <c:axId val="2048435288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7169,7 +7171,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028691176"/>
+        <c:crossAx val="-2067621688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7391,11 +7393,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028724856"/>
-        <c:axId val="-2028727608"/>
+        <c:axId val="-2067545288"/>
+        <c:axId val="-2067542392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028724856"/>
+        <c:axId val="-2067545288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7405,12 +7407,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028727608"/>
+        <c:crossAx val="-2067542392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028727608"/>
+        <c:axId val="-2067542392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7421,7 +7423,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028724856"/>
+        <c:crossAx val="-2067545288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7671,11 +7673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094674696"/>
-        <c:axId val="-2094677448"/>
+        <c:axId val="-2059811336"/>
+        <c:axId val="-2059808472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094674696"/>
+        <c:axId val="-2059811336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7685,12 +7687,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094677448"/>
+        <c:crossAx val="-2059808472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094677448"/>
+        <c:axId val="-2059808472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7701,14 +7703,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094674696"/>
+        <c:crossAx val="-2059811336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7884,11 +7885,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094710952"/>
-        <c:axId val="-2094713704"/>
+        <c:axId val="-2059926552"/>
+        <c:axId val="-2059923624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094710952"/>
+        <c:axId val="-2059926552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7898,12 +7899,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094713704"/>
+        <c:crossAx val="-2059923624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094713704"/>
+        <c:axId val="-2059923624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7914,14 +7915,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094710952"/>
+        <c:crossAx val="-2059926552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8097,11 +8097,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094744120"/>
-        <c:axId val="-2094746872"/>
+        <c:axId val="-2059893384"/>
+        <c:axId val="-2059890456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094744120"/>
+        <c:axId val="-2059893384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8111,12 +8111,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094746872"/>
+        <c:crossAx val="-2059890456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094746872"/>
+        <c:axId val="-2059890456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8127,14 +8127,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094744120"/>
+        <c:crossAx val="-2059893384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8371,11 +8370,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094777656"/>
-        <c:axId val="-2094780408"/>
+        <c:axId val="-2059859784"/>
+        <c:axId val="-2059856888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094777656"/>
+        <c:axId val="-2059859784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8385,12 +8384,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094780408"/>
+        <c:crossAx val="-2059856888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094780408"/>
+        <c:axId val="-2059856888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8401,14 +8400,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094777656"/>
+        <c:crossAx val="-2059859784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8645,11 +8643,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2029252872"/>
-        <c:axId val="-2029245944"/>
+        <c:axId val="-2071472120"/>
+        <c:axId val="-2071423480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2029252872"/>
+        <c:axId val="-2071472120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8659,12 +8657,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029245944"/>
+        <c:crossAx val="-2071423480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2029245944"/>
+        <c:axId val="-2071423480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8675,14 +8673,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029252872"/>
+        <c:crossAx val="-2071472120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8829,11 +8826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2029466600"/>
-        <c:axId val="-2029463816"/>
+        <c:axId val="-2071356168"/>
+        <c:axId val="-2071436392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2029466600"/>
+        <c:axId val="-2071356168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8843,12 +8840,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029463816"/>
+        <c:crossAx val="-2071436392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2029463816"/>
+        <c:axId val="-2071436392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8859,7 +8856,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029466600"/>
+        <c:crossAx val="-2071356168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9108,11 +9105,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2019832808"/>
-        <c:axId val="-2019830024"/>
+        <c:axId val="-2061779240"/>
+        <c:axId val="-2061776344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2019832808"/>
+        <c:axId val="-2061779240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9122,12 +9119,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019830024"/>
+        <c:crossAx val="-2061776344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2019830024"/>
+        <c:axId val="-2061776344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9138,14 +9135,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019832808"/>
+        <c:crossAx val="-2061779240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9321,11 +9317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2023513688"/>
-        <c:axId val="-2023516456"/>
+        <c:axId val="-2123348552"/>
+        <c:axId val="-2123345624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2023513688"/>
+        <c:axId val="-2123348552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9335,12 +9331,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2023516456"/>
+        <c:crossAx val="-2123345624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2023516456"/>
+        <c:axId val="-2123345624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9351,14 +9347,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2023513688"/>
+        <c:crossAx val="-2123348552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9534,11 +9529,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2021800552"/>
-        <c:axId val="-2021844376"/>
+        <c:axId val="-2062828408"/>
+        <c:axId val="-2062004504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2021800552"/>
+        <c:axId val="-2062828408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9548,12 +9543,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021844376"/>
+        <c:crossAx val="-2062004504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2021844376"/>
+        <c:axId val="-2062004504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9564,7 +9559,1564 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021800552"/>
+        <c:crossAx val="-2062828408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v4.1'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v4.1'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v4.1'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>205.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v4.1'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.286665786441329"/>
+                  <c:y val="0.0219323609139022"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v4.1'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v4.1'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>205.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>230.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2050524040"/>
+        <c:axId val="2123706216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2050524040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2123706216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2123706216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2050524040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v4.1'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0579260404949381"/>
+                  <c:y val="0.028316961194183"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v4.1'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>205.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v4.1'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2064134072"/>
+        <c:axId val="-2064131144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2064134072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2064131144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2064131144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2064134072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels v4.1'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.123849409448819"/>
+                  <c:y val="0.0421526584421247"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.00000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels v4.1'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>205.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>230.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels v4.1'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2061930040"/>
+        <c:axId val="-2061927112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2061930040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2061927112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2061927112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2061930040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0551179602549681"/>
+          <c:y val="0.0509259259259259"/>
+          <c:w val="0.764893888263967"/>
+          <c:h val="0.822469378827647"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lift v4.1'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UpSpeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lift v4.1'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lift v4.1'!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lift v4.1'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DownSpeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lift v4.1'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lift v4.1'!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2067608472"/>
+        <c:axId val="-2067605432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2067608472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2067605432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2067605432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2067608472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>UpPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0612814489349052"/>
+          <c:y val="0.18020202020202"/>
+          <c:w val="0.715281680950102"/>
+          <c:h val="0.713347013441502"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lift v4.1'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UpSpeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.121455315323154"/>
+                  <c:y val="0.0272778175455341"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lift v4.1'!$B$5:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lift v4.1'!$A$5:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2065140072"/>
+        <c:axId val="-2065154856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2065140072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2065154856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2065154856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2065140072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>DownPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0612814489349052"/>
+          <c:y val="0.18020202020202"/>
+          <c:w val="0.715281680950102"/>
+          <c:h val="0.713347013441502"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lift v4.1'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DownSpeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.121455315323154"/>
+                  <c:y val="0.0272778175455341"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lift v4.1'!$C$5:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lift v4.1'!$A$5:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2059505592"/>
+        <c:axId val="-2059502808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2059505592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2059502808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2059502808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2059505592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9826,11 +11378,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028415944"/>
-        <c:axId val="-2028413016"/>
+        <c:axId val="-2067790952"/>
+        <c:axId val="-2067787912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028415944"/>
+        <c:axId val="-2067790952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9840,12 +11392,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028413016"/>
+        <c:crossAx val="-2067787912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028413016"/>
+        <c:axId val="-2067787912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9856,7 +11408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028415944"/>
+        <c:crossAx val="-2067790952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10015,11 +11567,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028385240"/>
-        <c:axId val="-2028382456"/>
+        <c:axId val="-2062809864"/>
+        <c:axId val="-2062806968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028385240"/>
+        <c:axId val="-2062809864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10029,12 +11581,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028382456"/>
+        <c:crossAx val="-2062806968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028382456"/>
+        <c:axId val="-2062806968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10045,7 +11597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028385240"/>
+        <c:crossAx val="-2062809864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10198,11 +11750,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028352744"/>
-        <c:axId val="-2028349960"/>
+        <c:axId val="2124569944"/>
+        <c:axId val="2124572840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028352744"/>
+        <c:axId val="2124569944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10212,12 +11764,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028349960"/>
+        <c:crossAx val="2124572840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028349960"/>
+        <c:axId val="2124572840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10228,7 +11780,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028352744"/>
+        <c:crossAx val="2124569944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10453,11 +12005,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094069016"/>
-        <c:axId val="-2094066088"/>
+        <c:axId val="-2062905864"/>
+        <c:axId val="-2067729704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094069016"/>
+        <c:axId val="-2062905864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10467,12 +12019,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094066088"/>
+        <c:crossAx val="-2067729704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094066088"/>
+        <c:axId val="-2067729704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10483,7 +12035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094069016"/>
+        <c:crossAx val="-2062905864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10624,11 +12176,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094038424"/>
-        <c:axId val="-2094035640"/>
+        <c:axId val="-2067786072"/>
+        <c:axId val="-2067783176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094038424"/>
+        <c:axId val="-2067786072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10638,12 +12190,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094035640"/>
+        <c:crossAx val="-2067783176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094035640"/>
+        <c:axId val="-2067783176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10654,7 +12206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094038424"/>
+        <c:crossAx val="-2067786072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11084,6 +12636,208 @@
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13207,7 +14961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -13333,6 +15087,366 @@
       <c r="C11">
         <v>249</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>96</v>
+      </c>
+      <c r="C5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>130</v>
+      </c>
+      <c r="C6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>155</v>
+      </c>
+      <c r="C7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>181</v>
+      </c>
+      <c r="C8">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>205</v>
+      </c>
+      <c r="C9">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>235</v>
+      </c>
+      <c r="C10">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>1.3</v>
+      </c>
+      <c r="C3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.25</v>
+      </c>
+      <c r="B4">
+        <v>1.8</v>
+      </c>
+      <c r="C4">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.3</v>
+      </c>
+      <c r="B5">
+        <v>1.9</v>
+      </c>
+      <c r="C5">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.35</v>
+      </c>
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.4</v>
+      </c>
+      <c r="B7">
+        <v>3.2</v>
+      </c>
+      <c r="C7">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.45</v>
+      </c>
+      <c r="B8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C8">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B10">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>0.6</v>
+      </c>
+      <c r="B11">
+        <v>7.1</v>
+      </c>
+      <c r="C11">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>0.65</v>
+      </c>
+      <c r="B12">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>0.7</v>
+      </c>
+      <c r="B13">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C13">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>0.75</v>
+      </c>
+      <c r="B14">
+        <v>8.9</v>
+      </c>
+      <c r="C14">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>0.8</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>0.85</v>
+      </c>
+      <c r="B16">
+        <v>9.1</v>
+      </c>
+      <c r="C16">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>0.9</v>
+      </c>
+      <c r="C17">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>0.95000000000000095</v>
+      </c>
+      <c r="B18">
+        <v>10.9</v>
+      </c>
+      <c r="C18">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Consolidated controller gains for both wheels
</commit_message>
<xml_diff>
--- a/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
+++ b/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="39640" yWindow="0" windowWidth="35160" windowHeight="19580" tabRatio="500" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="860" yWindow="0" windowWidth="35160" windowHeight="19580" tabRatio="500" firstSheet="8" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Wheels" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Wheels v4" sheetId="12" r:id="rId12"/>
     <sheet name="Wheels v4.1" sheetId="13" r:id="rId13"/>
     <sheet name="Lift v4.1" sheetId="14" r:id="rId14"/>
+    <sheet name="Wheels EP1" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="16">
   <si>
     <t>Power</t>
   </si>
@@ -74,6 +75,12 @@
   </si>
   <si>
     <t>MAX_WHEEL_SPEED = 0.75</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>EP1-F</t>
   </si>
 </sst>
 </file>
@@ -474,11 +481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2126498824"/>
-        <c:axId val="-2064074696"/>
+        <c:axId val="-2093824520"/>
+        <c:axId val="-2093818616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2126498824"/>
+        <c:axId val="-2093824520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,12 +495,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064074696"/>
+        <c:crossAx val="-2093818616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2064074696"/>
+        <c:axId val="-2093818616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -504,7 +511,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126498824"/>
+        <c:crossAx val="-2093824520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -639,11 +646,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2063157864"/>
-        <c:axId val="2048445528"/>
+        <c:axId val="-2093676264"/>
+        <c:axId val="-2093673480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2063157864"/>
+        <c:axId val="-2093676264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,12 +660,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048445528"/>
+        <c:crossAx val="-2093673480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2048445528"/>
+        <c:axId val="-2093673480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +676,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063157864"/>
+        <c:crossAx val="-2093676264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -918,11 +925,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062785400"/>
-        <c:axId val="-2063200680"/>
+        <c:axId val="-2093624984"/>
+        <c:axId val="-2093622056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062785400"/>
+        <c:axId val="-2093624984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -932,12 +939,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063200680"/>
+        <c:crossAx val="-2093622056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2063200680"/>
+        <c:axId val="-2093622056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,7 +955,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062785400"/>
+        <c:crossAx val="-2093624984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1101,11 +1108,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2063212408"/>
-        <c:axId val="-2063210184"/>
+        <c:axId val="-2093594152"/>
+        <c:axId val="-2093591368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2063212408"/>
+        <c:axId val="-2093594152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1115,12 +1122,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063210184"/>
+        <c:crossAx val="-2093591368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2063210184"/>
+        <c:axId val="-2093591368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,7 +1138,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063212408"/>
+        <c:crossAx val="-2093594152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1278,11 +1285,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2123290504"/>
-        <c:axId val="-2123287608"/>
+        <c:axId val="-2093561384"/>
+        <c:axId val="-2093558600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2123290504"/>
+        <c:axId val="-2093561384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,12 +1299,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123287608"/>
+        <c:crossAx val="-2093558600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123287608"/>
+        <c:axId val="-2093558600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123290504"/>
+        <c:crossAx val="-2093561384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1600,11 +1607,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122466040"/>
-        <c:axId val="-2122488136"/>
+        <c:axId val="-2093511784"/>
+        <c:axId val="-2093509000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122466040"/>
+        <c:axId val="-2093511784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1614,12 +1621,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122488136"/>
+        <c:crossAx val="-2093509000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122488136"/>
+        <c:axId val="-2093509000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122466040"/>
+        <c:crossAx val="-2093511784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1838,11 +1845,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059792344"/>
-        <c:axId val="-2059789384"/>
+        <c:axId val="-2093479608"/>
+        <c:axId val="-2093476760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059792344"/>
+        <c:axId val="-2093479608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,12 +1859,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059789384"/>
+        <c:crossAx val="-2093476760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059789384"/>
+        <c:axId val="-2093476760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1868,7 +1875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059792344"/>
+        <c:crossAx val="-2093479608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2070,11 +2077,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059995096"/>
-        <c:axId val="-2059996920"/>
+        <c:axId val="-2093445448"/>
+        <c:axId val="-2093442696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059995096"/>
+        <c:axId val="-2093445448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2084,12 +2091,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059996920"/>
+        <c:crossAx val="-2093442696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059996920"/>
+        <c:axId val="-2093442696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2100,7 +2107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059995096"/>
+        <c:crossAx val="-2093445448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2379,11 +2386,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2047556136"/>
-        <c:axId val="2047559032"/>
+        <c:axId val="-2093410920"/>
+        <c:axId val="-2093408136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2047556136"/>
+        <c:axId val="-2093410920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2393,12 +2400,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047559032"/>
+        <c:crossAx val="-2093408136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2047559032"/>
+        <c:axId val="-2093408136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2409,7 +2416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047556136"/>
+        <c:crossAx val="-2093410920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2682,11 +2689,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059827224"/>
-        <c:axId val="-2059824328"/>
+        <c:axId val="-2093376888"/>
+        <c:axId val="-2093374104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059827224"/>
+        <c:axId val="-2093376888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2696,12 +2703,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059824328"/>
+        <c:crossAx val="-2093374104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059824328"/>
+        <c:axId val="-2093374104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2712,7 +2719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059827224"/>
+        <c:crossAx val="-2093376888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3004,11 +3011,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2071545752"/>
-        <c:axId val="-2063735064"/>
+        <c:axId val="-2093327224"/>
+        <c:axId val="-2093324440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2071545752"/>
+        <c:axId val="-2093327224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3018,12 +3025,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063735064"/>
+        <c:crossAx val="-2093324440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2063735064"/>
+        <c:axId val="-2093324440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3034,7 +3041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071545752"/>
+        <c:crossAx val="-2093327224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3193,11 +3200,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2064170312"/>
-        <c:axId val="-2063639048"/>
+        <c:axId val="-2094334040"/>
+        <c:axId val="-2094331256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2064170312"/>
+        <c:axId val="-2094334040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3207,12 +3214,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063639048"/>
+        <c:crossAx val="-2094331256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2063639048"/>
+        <c:axId val="-2094331256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3223,7 +3230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064170312"/>
+        <c:crossAx val="-2094334040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3431,11 +3438,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2063744568"/>
-        <c:axId val="-2063741640"/>
+        <c:axId val="-2093294568"/>
+        <c:axId val="-2093291816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2063744568"/>
+        <c:axId val="-2093294568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3445,12 +3452,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063741640"/>
+        <c:crossAx val="-2093291816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2063741640"/>
+        <c:axId val="-2093291816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3461,7 +3468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063744568"/>
+        <c:crossAx val="-2093294568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3663,11 +3670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2064144392"/>
-        <c:axId val="-2126456392"/>
+        <c:axId val="-2093261160"/>
+        <c:axId val="-2093258312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2064144392"/>
+        <c:axId val="-2093261160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3677,12 +3684,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126456392"/>
+        <c:crossAx val="-2093258312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2126456392"/>
+        <c:axId val="-2093258312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3693,7 +3700,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064144392"/>
+        <c:crossAx val="-2093261160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3972,11 +3979,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2063932184"/>
-        <c:axId val="-2063929288"/>
+        <c:axId val="-2093227160"/>
+        <c:axId val="-2093224376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2063932184"/>
+        <c:axId val="-2093227160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3986,12 +3993,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063929288"/>
+        <c:crossAx val="-2093224376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2063929288"/>
+        <c:axId val="-2093224376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4002,7 +4009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063932184"/>
+        <c:crossAx val="-2093227160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4275,11 +4282,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2064385400"/>
-        <c:axId val="-2064314344"/>
+        <c:axId val="-2093193304"/>
+        <c:axId val="-2093190520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2064385400"/>
+        <c:axId val="-2093193304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4289,12 +4296,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064314344"/>
+        <c:crossAx val="-2093190520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2064314344"/>
+        <c:axId val="-2093190520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4305,7 +4312,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064385400"/>
+        <c:crossAx val="-2093193304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4554,11 +4561,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2064193656"/>
-        <c:axId val="-2064190920"/>
+        <c:axId val="-2093141448"/>
+        <c:axId val="-2093138520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2064193656"/>
+        <c:axId val="-2093141448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4568,12 +4575,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064190920"/>
+        <c:crossAx val="-2093138520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2064190920"/>
+        <c:axId val="-2093138520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4584,7 +4591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064193656"/>
+        <c:crossAx val="-2093141448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4762,11 +4769,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2064160392"/>
-        <c:axId val="-2064157496"/>
+        <c:axId val="-2093109304"/>
+        <c:axId val="-2093106520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2064160392"/>
+        <c:axId val="-2093109304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4776,12 +4783,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064157496"/>
+        <c:crossAx val="-2093106520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2064157496"/>
+        <c:axId val="-2093106520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4792,7 +4799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064160392"/>
+        <c:crossAx val="-2093109304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4970,11 +4977,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2071392264"/>
-        <c:axId val="-2071389368"/>
+        <c:axId val="-2093076312"/>
+        <c:axId val="-2093073528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2071392264"/>
+        <c:axId val="-2093076312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4984,12 +4991,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071389368"/>
+        <c:crossAx val="-2093073528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2071389368"/>
+        <c:axId val="-2093073528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5000,7 +5007,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071392264"/>
+        <c:crossAx val="-2093076312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5249,11 +5256,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062008792"/>
-        <c:axId val="-2062110792"/>
+        <c:axId val="2133194680"/>
+        <c:axId val="2133201768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062008792"/>
+        <c:axId val="2133194680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5263,12 +5270,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062110792"/>
+        <c:crossAx val="2133201768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2062110792"/>
+        <c:axId val="2133201768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5279,7 +5286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062008792"/>
+        <c:crossAx val="2133194680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5461,11 +5468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123533960"/>
-        <c:axId val="2123724296"/>
+        <c:axId val="2132819496"/>
+        <c:axId val="2132821304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123533960"/>
+        <c:axId val="2132819496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5475,12 +5482,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123724296"/>
+        <c:crossAx val="2132821304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123724296"/>
+        <c:axId val="2132821304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5491,7 +5498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123533960"/>
+        <c:crossAx val="2132819496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5673,11 +5680,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061757560"/>
-        <c:axId val="-2123098376"/>
+        <c:axId val="-2092834328"/>
+        <c:axId val="-2092832296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061757560"/>
+        <c:axId val="-2092834328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5687,12 +5694,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123098376"/>
+        <c:crossAx val="-2092832296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123098376"/>
+        <c:axId val="-2092832296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5703,7 +5710,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061757560"/>
+        <c:crossAx val="-2092834328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5954,11 +5961,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2071975464"/>
-        <c:axId val="-2071972424"/>
+        <c:axId val="2133283016"/>
+        <c:axId val="2133281944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2071975464"/>
+        <c:axId val="2133283016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5968,12 +5975,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071972424"/>
+        <c:crossAx val="2133281944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2071972424"/>
+        <c:axId val="2133281944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5984,7 +5991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071975464"/>
+        <c:crossAx val="2133283016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6227,11 +6234,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062669512"/>
-        <c:axId val="-2063293016"/>
+        <c:axId val="-2092809800"/>
+        <c:axId val="-2092807624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062669512"/>
+        <c:axId val="-2092809800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6241,12 +6248,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063293016"/>
+        <c:crossAx val="-2092807624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2063293016"/>
+        <c:axId val="-2092807624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6257,7 +6264,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062669512"/>
+        <c:crossAx val="-2092809800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6500,11 +6507,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2067736616"/>
-        <c:axId val="-2067767400"/>
+        <c:axId val="-2092779928"/>
+        <c:axId val="-2092777144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2067736616"/>
+        <c:axId val="-2092779928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6514,12 +6521,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067767400"/>
+        <c:crossAx val="-2092777144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2067767400"/>
+        <c:axId val="-2092777144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6530,7 +6537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067736616"/>
+        <c:crossAx val="-2092779928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6605,7 +6612,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -6755,7 +6761,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -6889,11 +6894,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062609144"/>
-        <c:axId val="-2062773752"/>
+        <c:axId val="-2092720552"/>
+        <c:axId val="-2092717624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062609144"/>
+        <c:axId val="-2092720552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6903,12 +6908,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062773752"/>
+        <c:crossAx val="-2092717624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2062773752"/>
+        <c:axId val="-2092717624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6919,14 +6924,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062609144"/>
+        <c:crossAx val="-2092720552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6971,7 +6975,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7141,11 +7144,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2067621688"/>
-        <c:axId val="2048435288"/>
+        <c:axId val="-2095722568"/>
+        <c:axId val="2134038984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2067621688"/>
+        <c:axId val="-2095722568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7155,12 +7158,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048435288"/>
+        <c:crossAx val="2134038984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2048435288"/>
+        <c:axId val="2134038984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7171,14 +7174,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067621688"/>
+        <c:crossAx val="-2095722568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7223,7 +7225,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7393,11 +7394,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2067545288"/>
-        <c:axId val="-2067542392"/>
+        <c:axId val="-2092696808"/>
+        <c:axId val="2028237480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2067545288"/>
+        <c:axId val="-2092696808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7407,12 +7408,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067542392"/>
+        <c:crossAx val="2028237480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2067542392"/>
+        <c:axId val="2028237480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7423,14 +7424,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067545288"/>
+        <c:crossAx val="-2092696808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7673,11 +7673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059811336"/>
-        <c:axId val="-2059808472"/>
+        <c:axId val="2028269784"/>
+        <c:axId val="-2093435272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059811336"/>
+        <c:axId val="2028269784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7687,12 +7687,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059808472"/>
+        <c:crossAx val="-2093435272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059808472"/>
+        <c:axId val="-2093435272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7703,7 +7703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059811336"/>
+        <c:crossAx val="2028269784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7885,11 +7885,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059926552"/>
-        <c:axId val="-2059923624"/>
+        <c:axId val="2028351672"/>
+        <c:axId val="2028386712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059926552"/>
+        <c:axId val="2028351672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7899,12 +7899,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059923624"/>
+        <c:crossAx val="2028386712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059923624"/>
+        <c:axId val="2028386712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7915,7 +7915,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059926552"/>
+        <c:crossAx val="2028351672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8097,11 +8097,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059893384"/>
-        <c:axId val="-2059890456"/>
+        <c:axId val="2028357384"/>
+        <c:axId val="2028360312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059893384"/>
+        <c:axId val="2028357384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8111,12 +8111,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059890456"/>
+        <c:crossAx val="2028360312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059890456"/>
+        <c:axId val="2028360312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8127,7 +8127,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059893384"/>
+        <c:crossAx val="2028357384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8370,11 +8370,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059859784"/>
-        <c:axId val="-2059856888"/>
+        <c:axId val="2028261624"/>
+        <c:axId val="2028264328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059859784"/>
+        <c:axId val="2028261624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8384,12 +8384,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059856888"/>
+        <c:crossAx val="2028264328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059856888"/>
+        <c:axId val="2028264328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8400,7 +8400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059859784"/>
+        <c:crossAx val="2028261624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8643,11 +8643,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2071472120"/>
-        <c:axId val="-2071423480"/>
+        <c:axId val="2028340552"/>
+        <c:axId val="2028301976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2071472120"/>
+        <c:axId val="2028340552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8657,12 +8657,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071423480"/>
+        <c:crossAx val="2028301976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2071423480"/>
+        <c:axId val="2028301976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8673,7 +8673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071472120"/>
+        <c:crossAx val="2028340552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8826,11 +8826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2071356168"/>
-        <c:axId val="-2071436392"/>
+        <c:axId val="2133214712"/>
+        <c:axId val="2133206648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2071356168"/>
+        <c:axId val="2133214712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8840,12 +8840,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071436392"/>
+        <c:crossAx val="2133206648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2071436392"/>
+        <c:axId val="2133206648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8856,7 +8856,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071356168"/>
+        <c:crossAx val="2133214712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9105,11 +9105,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061779240"/>
-        <c:axId val="-2061776344"/>
+        <c:axId val="-2093022360"/>
+        <c:axId val="-2093019576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061779240"/>
+        <c:axId val="-2093022360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9119,12 +9119,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061776344"/>
+        <c:crossAx val="-2093019576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2061776344"/>
+        <c:axId val="-2093019576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9135,7 +9135,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061779240"/>
+        <c:crossAx val="-2093022360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9317,11 +9317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2123348552"/>
-        <c:axId val="-2123345624"/>
+        <c:axId val="-2092990280"/>
+        <c:axId val="-2092987528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2123348552"/>
+        <c:axId val="-2092990280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9331,12 +9331,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123345624"/>
+        <c:crossAx val="-2092987528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123345624"/>
+        <c:axId val="-2092987528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9347,7 +9347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123348552"/>
+        <c:crossAx val="-2092990280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9529,11 +9529,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062828408"/>
-        <c:axId val="-2062004504"/>
+        <c:axId val="2116604840"/>
+        <c:axId val="-2095726088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062828408"/>
+        <c:axId val="2116604840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9543,12 +9543,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062004504"/>
+        <c:crossAx val="-2095726088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2062004504"/>
+        <c:axId val="-2095726088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9559,7 +9559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062828408"/>
+        <c:crossAx val="2116604840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9802,11 +9802,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2050524040"/>
-        <c:axId val="2123706216"/>
+        <c:axId val="-2095447624"/>
+        <c:axId val="-2095444840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2050524040"/>
+        <c:axId val="-2095447624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9816,12 +9816,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123706216"/>
+        <c:crossAx val="-2095444840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123706216"/>
+        <c:axId val="-2095444840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9832,7 +9832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050524040"/>
+        <c:crossAx val="-2095447624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10012,11 +10012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2064134072"/>
-        <c:axId val="-2064131144"/>
+        <c:axId val="-2095415912"/>
+        <c:axId val="-2095413144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2064134072"/>
+        <c:axId val="-2095415912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10026,12 +10026,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064131144"/>
+        <c:crossAx val="-2095413144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2064131144"/>
+        <c:axId val="-2095413144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10042,7 +10042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064134072"/>
+        <c:crossAx val="-2095415912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10222,11 +10222,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061930040"/>
-        <c:axId val="-2061927112"/>
+        <c:axId val="-2095382712"/>
+        <c:axId val="-2095379944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061930040"/>
+        <c:axId val="-2095382712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10236,12 +10236,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061927112"/>
+        <c:crossAx val="-2095379944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2061927112"/>
+        <c:axId val="-2095379944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10252,7 +10252,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061930040"/>
+        <c:crossAx val="-2095382712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10597,11 +10597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2067608472"/>
-        <c:axId val="-2067605432"/>
+        <c:axId val="-2095332744"/>
+        <c:axId val="-2095329816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2067608472"/>
+        <c:axId val="-2095332744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10611,12 +10611,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067605432"/>
+        <c:crossAx val="-2095329816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2067605432"/>
+        <c:axId val="-2095329816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10627,7 +10627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067608472"/>
+        <c:crossAx val="-2095332744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10843,11 +10843,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2065140072"/>
-        <c:axId val="-2065154856"/>
+        <c:axId val="-2095301160"/>
+        <c:axId val="-2095298376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2065140072"/>
+        <c:axId val="-2095301160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10857,12 +10857,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2065154856"/>
+        <c:crossAx val="-2095298376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2065154856"/>
+        <c:axId val="-2095298376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10873,7 +10873,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2065140072"/>
+        <c:crossAx val="-2095301160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11086,11 +11086,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059505592"/>
-        <c:axId val="-2059502808"/>
+        <c:axId val="-2093005432"/>
+        <c:axId val="-2092979864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059505592"/>
+        <c:axId val="-2093005432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11100,12 +11100,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059502808"/>
+        <c:crossAx val="-2092979864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2059502808"/>
+        <c:axId val="-2092979864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11116,7 +11116,281 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059505592"/>
+        <c:crossAx val="-2093005432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels EP1'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels EP1'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels EP1'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>187.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels EP1'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.286665786441329"/>
+                  <c:y val="0.0219323609139022"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels EP1'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels EP1'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>195.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>227.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>254.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2090030152"/>
+        <c:axId val="-2090027368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2090030152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2090027368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2090027368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2090030152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11378,11 +11652,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2067790952"/>
-        <c:axId val="-2067787912"/>
+        <c:axId val="2133140504"/>
+        <c:axId val="2133143432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2067790952"/>
+        <c:axId val="2133140504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11392,12 +11666,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067787912"/>
+        <c:crossAx val="2133143432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2067787912"/>
+        <c:axId val="2133143432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11408,13 +11682,433 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067790952"/>
+        <c:crossAx val="2133140504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels EP1'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0579260404949381"/>
+                  <c:y val="0.028316961194183"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels EP1'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>187.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels EP1'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2090000872"/>
+        <c:axId val="-2089998120"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2090000872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2089998120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2089998120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2090000872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels EP1'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.123849409448819"/>
+                  <c:y val="0.0421526584421247"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.00000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels EP1'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>195.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>227.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>254.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels EP1'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2089016680"/>
+        <c:axId val="-2088978424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2089016680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2088978424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2088978424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2089016680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11567,11 +12261,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062809864"/>
-        <c:axId val="-2062806968"/>
+        <c:axId val="2132915960"/>
+        <c:axId val="2132892920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062809864"/>
+        <c:axId val="2132915960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11581,12 +12275,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062806968"/>
+        <c:crossAx val="2132892920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2062806968"/>
+        <c:axId val="2132892920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11597,7 +12291,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062809864"/>
+        <c:crossAx val="2132915960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11750,11 +12444,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2124569944"/>
-        <c:axId val="2124572840"/>
+        <c:axId val="2132840200"/>
+        <c:axId val="2132843096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2124569944"/>
+        <c:axId val="2132840200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11764,12 +12458,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124572840"/>
+        <c:crossAx val="2132843096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2124572840"/>
+        <c:axId val="2132843096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11780,7 +12474,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124569944"/>
+        <c:crossAx val="2132840200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12005,11 +12699,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062905864"/>
-        <c:axId val="-2067729704"/>
+        <c:axId val="-2093740264"/>
+        <c:axId val="-2093737336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062905864"/>
+        <c:axId val="-2093740264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12019,12 +12713,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067729704"/>
+        <c:crossAx val="-2093737336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2067729704"/>
+        <c:axId val="-2093737336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12035,7 +12729,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062905864"/>
+        <c:crossAx val="-2093740264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12176,11 +12870,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2067786072"/>
-        <c:axId val="-2067783176"/>
+        <c:axId val="-2093709624"/>
+        <c:axId val="-2093706840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2067786072"/>
+        <c:axId val="-2093709624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12190,12 +12884,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067783176"/>
+        <c:crossAx val="-2093706840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2067783176"/>
+        <c:axId val="-2093706840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12206,7 +12900,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067786072"/>
+        <c:crossAx val="-2093709624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12838,6 +13532,107 @@
       <xdr:colOff>139700</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15241,7 +16036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -15447,6 +16242,153 @@
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>62</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>120</v>
+      </c>
+      <c r="C6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>157</v>
+      </c>
+      <c r="C7">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>187</v>
+      </c>
+      <c r="C8">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>220</v>
+      </c>
+      <c r="C9">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>235</v>
+      </c>
+      <c r="C10">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Wheels retuned for EP2
</commit_message>
<xml_diff>
--- a/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
+++ b/tools/controller_tuning/wheel-power-speed-worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="0" windowWidth="35160" windowHeight="19580" tabRatio="500" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="860" yWindow="0" windowWidth="35160" windowHeight="19580" tabRatio="500" firstSheet="9" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Wheels" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Wheels v4.1" sheetId="13" r:id="rId13"/>
     <sheet name="Lift v4.1" sheetId="14" r:id="rId14"/>
     <sheet name="Wheels EP1" sheetId="16" r:id="rId15"/>
+    <sheet name="Wheels EP2" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="17">
   <si>
     <t>Power</t>
   </si>
@@ -81,6 +82,9 @@
   </si>
   <si>
     <t>EP1-F</t>
+  </si>
+  <si>
+    <t>EP2 - 015e</t>
   </si>
 </sst>
 </file>
@@ -481,11 +485,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093824520"/>
-        <c:axId val="-2093818616"/>
+        <c:axId val="-2120964248"/>
+        <c:axId val="-2120978712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093824520"/>
+        <c:axId val="-2120964248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,12 +499,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093818616"/>
+        <c:crossAx val="-2120978712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093818616"/>
+        <c:axId val="-2120978712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -511,7 +515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093824520"/>
+        <c:crossAx val="-2120964248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -646,11 +650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093676264"/>
-        <c:axId val="-2093673480"/>
+        <c:axId val="-2121101608"/>
+        <c:axId val="-2121104360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093676264"/>
+        <c:axId val="-2121101608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,12 +664,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093673480"/>
+        <c:crossAx val="-2121104360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093673480"/>
+        <c:axId val="-2121104360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093676264"/>
+        <c:crossAx val="-2121101608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -925,11 +929,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093624984"/>
-        <c:axId val="-2093622056"/>
+        <c:axId val="-2121160712"/>
+        <c:axId val="-2121163608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093624984"/>
+        <c:axId val="-2121160712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,12 +943,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093622056"/>
+        <c:crossAx val="-2121163608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093622056"/>
+        <c:axId val="-2121163608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093624984"/>
+        <c:crossAx val="-2121160712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1108,11 +1112,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093594152"/>
-        <c:axId val="-2093591368"/>
+        <c:axId val="-2121191544"/>
+        <c:axId val="-2121194296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093594152"/>
+        <c:axId val="-2121191544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,12 +1126,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093591368"/>
+        <c:crossAx val="-2121194296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093591368"/>
+        <c:axId val="-2121194296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,7 +1142,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093594152"/>
+        <c:crossAx val="-2121191544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1285,11 +1289,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093561384"/>
-        <c:axId val="-2093558600"/>
+        <c:axId val="-2121224312"/>
+        <c:axId val="-2121227064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093561384"/>
+        <c:axId val="-2121224312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,12 +1303,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093558600"/>
+        <c:crossAx val="-2121227064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093558600"/>
+        <c:axId val="-2121227064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,7 +1319,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093561384"/>
+        <c:crossAx val="-2121224312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1607,11 +1611,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093511784"/>
-        <c:axId val="-2093509000"/>
+        <c:axId val="-2078866632"/>
+        <c:axId val="-2078863848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093511784"/>
+        <c:axId val="-2078866632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,12 +1625,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093509000"/>
+        <c:crossAx val="-2078863848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093509000"/>
+        <c:axId val="-2078863848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093511784"/>
+        <c:crossAx val="-2078866632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1845,11 +1849,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093479608"/>
-        <c:axId val="-2093476760"/>
+        <c:axId val="-2114498136"/>
+        <c:axId val="-2114495288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093479608"/>
+        <c:axId val="-2114498136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1859,12 +1863,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093476760"/>
+        <c:crossAx val="-2114495288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093476760"/>
+        <c:axId val="-2114495288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1879,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093479608"/>
+        <c:crossAx val="-2114498136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2077,11 +2081,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093445448"/>
-        <c:axId val="-2093442696"/>
+        <c:axId val="-2114459064"/>
+        <c:axId val="-2114456312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093445448"/>
+        <c:axId val="-2114459064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2091,12 +2095,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093442696"/>
+        <c:crossAx val="-2114456312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093442696"/>
+        <c:axId val="-2114456312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2107,7 +2111,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093445448"/>
+        <c:crossAx val="-2114459064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2386,11 +2390,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093410920"/>
-        <c:axId val="-2093408136"/>
+        <c:axId val="-2078836152"/>
+        <c:axId val="-2078833368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093410920"/>
+        <c:axId val="-2078836152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,12 +2404,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093408136"/>
+        <c:crossAx val="-2078833368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093408136"/>
+        <c:axId val="-2078833368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2416,7 +2420,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093410920"/>
+        <c:crossAx val="-2078836152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2689,11 +2693,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093376888"/>
-        <c:axId val="-2093374104"/>
+        <c:axId val="-2078798600"/>
+        <c:axId val="-2078795816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093376888"/>
+        <c:axId val="-2078798600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2703,12 +2707,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093374104"/>
+        <c:crossAx val="-2078795816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093374104"/>
+        <c:axId val="-2078795816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2719,7 +2723,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093376888"/>
+        <c:crossAx val="-2078798600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3011,11 +3015,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093327224"/>
-        <c:axId val="-2093324440"/>
+        <c:axId val="2060284264"/>
+        <c:axId val="2060287048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093327224"/>
+        <c:axId val="2060284264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,12 +3029,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093324440"/>
+        <c:crossAx val="2060287048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093324440"/>
+        <c:axId val="2060287048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3041,7 +3045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093327224"/>
+        <c:crossAx val="2060284264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3200,11 +3204,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094334040"/>
-        <c:axId val="-2094331256"/>
+        <c:axId val="-2079907240"/>
+        <c:axId val="-2079904456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094334040"/>
+        <c:axId val="-2079907240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3214,12 +3218,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094331256"/>
+        <c:crossAx val="-2079904456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094331256"/>
+        <c:axId val="-2079904456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3230,7 +3234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094334040"/>
+        <c:crossAx val="-2079907240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3438,11 +3442,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093294568"/>
-        <c:axId val="-2093291816"/>
+        <c:axId val="-2116986808"/>
+        <c:axId val="-2116995128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093294568"/>
+        <c:axId val="-2116986808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3452,12 +3456,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093291816"/>
+        <c:crossAx val="-2116995128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093291816"/>
+        <c:axId val="-2116995128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3468,7 +3472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093294568"/>
+        <c:crossAx val="-2116986808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3670,11 +3674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093261160"/>
-        <c:axId val="-2093258312"/>
+        <c:axId val="-2117033128"/>
+        <c:axId val="-2117035944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093261160"/>
+        <c:axId val="-2117033128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3684,12 +3688,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093258312"/>
+        <c:crossAx val="-2117035944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093258312"/>
+        <c:axId val="-2117035944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3700,7 +3704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093261160"/>
+        <c:crossAx val="-2117033128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3979,11 +3983,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093227160"/>
-        <c:axId val="-2093224376"/>
+        <c:axId val="-2117067128"/>
+        <c:axId val="-2117069880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093227160"/>
+        <c:axId val="-2117067128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3993,12 +3997,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093224376"/>
+        <c:crossAx val="-2117069880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093224376"/>
+        <c:axId val="-2117069880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4009,7 +4013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093227160"/>
+        <c:crossAx val="-2117067128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4282,11 +4286,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093193304"/>
-        <c:axId val="-2093190520"/>
+        <c:axId val="-2077816008"/>
+        <c:axId val="-2077810616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093193304"/>
+        <c:axId val="-2077816008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4296,12 +4300,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093190520"/>
+        <c:crossAx val="-2077810616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093190520"/>
+        <c:axId val="-2077810616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4312,7 +4316,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093193304"/>
+        <c:crossAx val="-2077816008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4561,11 +4565,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093141448"/>
-        <c:axId val="-2093138520"/>
+        <c:axId val="-2121216888"/>
+        <c:axId val="-2078778216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093141448"/>
+        <c:axId val="-2121216888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4575,12 +4579,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093138520"/>
+        <c:crossAx val="-2078778216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093138520"/>
+        <c:axId val="-2078778216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4591,7 +4595,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093141448"/>
+        <c:crossAx val="-2121216888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4769,11 +4773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093109304"/>
-        <c:axId val="-2093106520"/>
+        <c:axId val="-2077752136"/>
+        <c:axId val="-2077749352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093109304"/>
+        <c:axId val="-2077752136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4783,12 +4787,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093106520"/>
+        <c:crossAx val="-2077749352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093106520"/>
+        <c:axId val="-2077749352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4799,7 +4803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093109304"/>
+        <c:crossAx val="-2077752136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4977,11 +4981,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093076312"/>
-        <c:axId val="-2093073528"/>
+        <c:axId val="-2077714168"/>
+        <c:axId val="-2077711384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093076312"/>
+        <c:axId val="-2077714168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4991,12 +4995,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093073528"/>
+        <c:crossAx val="-2077711384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093073528"/>
+        <c:axId val="-2077711384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5007,7 +5011,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093076312"/>
+        <c:crossAx val="-2077714168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5256,11 +5260,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2133194680"/>
-        <c:axId val="2133201768"/>
+        <c:axId val="-2078726760"/>
+        <c:axId val="-2078723976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2133194680"/>
+        <c:axId val="-2078726760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5270,12 +5274,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133201768"/>
+        <c:crossAx val="-2078723976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2133201768"/>
+        <c:axId val="-2078723976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5286,7 +5290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133194680"/>
+        <c:crossAx val="-2078726760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5468,11 +5472,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2132819496"/>
-        <c:axId val="2132821304"/>
+        <c:axId val="-2078694152"/>
+        <c:axId val="-2078691400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2132819496"/>
+        <c:axId val="-2078694152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5482,12 +5486,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132821304"/>
+        <c:crossAx val="-2078691400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2132821304"/>
+        <c:axId val="-2078691400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5498,7 +5502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132819496"/>
+        <c:crossAx val="-2078694152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5680,11 +5684,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092834328"/>
-        <c:axId val="-2092832296"/>
+        <c:axId val="-2078661080"/>
+        <c:axId val="-2078658328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092834328"/>
+        <c:axId val="-2078661080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5694,12 +5698,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092832296"/>
+        <c:crossAx val="-2078658328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092832296"/>
+        <c:axId val="-2078658328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5710,7 +5714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092834328"/>
+        <c:crossAx val="-2078661080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5961,11 +5965,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2133283016"/>
-        <c:axId val="2133281944"/>
+        <c:axId val="-2116814056"/>
+        <c:axId val="-2116816952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2133283016"/>
+        <c:axId val="-2116814056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5975,12 +5979,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133281944"/>
+        <c:crossAx val="-2116816952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2133281944"/>
+        <c:axId val="-2116816952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5991,7 +5995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133283016"/>
+        <c:crossAx val="-2116814056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6234,11 +6238,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092809800"/>
-        <c:axId val="-2092807624"/>
+        <c:axId val="-2078627080"/>
+        <c:axId val="-2078624296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092809800"/>
+        <c:axId val="-2078627080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6248,12 +6252,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092807624"/>
+        <c:crossAx val="-2078624296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092807624"/>
+        <c:axId val="-2078624296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6264,7 +6268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092809800"/>
+        <c:crossAx val="-2078627080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6507,11 +6511,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092779928"/>
-        <c:axId val="-2092777144"/>
+        <c:axId val="-2078593256"/>
+        <c:axId val="-2078590472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092779928"/>
+        <c:axId val="-2078593256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6521,12 +6525,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092777144"/>
+        <c:crossAx val="-2078590472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092777144"/>
+        <c:axId val="-2078590472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6537,7 +6541,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092779928"/>
+        <c:crossAx val="-2078593256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6894,11 +6898,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092720552"/>
-        <c:axId val="-2092717624"/>
+        <c:axId val="-2114423976"/>
+        <c:axId val="-2114421048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092720552"/>
+        <c:axId val="-2114423976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6908,12 +6912,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092717624"/>
+        <c:crossAx val="-2114421048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092717624"/>
+        <c:axId val="-2114421048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6924,7 +6928,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092720552"/>
+        <c:crossAx val="-2114423976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7144,11 +7148,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2095722568"/>
-        <c:axId val="2134038984"/>
+        <c:axId val="-2114388008"/>
+        <c:axId val="-2114385224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2095722568"/>
+        <c:axId val="-2114388008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7158,12 +7162,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134038984"/>
+        <c:crossAx val="-2114385224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2134038984"/>
+        <c:axId val="-2114385224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7174,7 +7178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095722568"/>
+        <c:crossAx val="-2114388008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7394,11 +7398,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092696808"/>
-        <c:axId val="2028237480"/>
+        <c:axId val="-2114354040"/>
+        <c:axId val="-2114351256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092696808"/>
+        <c:axId val="-2114354040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7408,12 +7412,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028237480"/>
+        <c:crossAx val="-2114351256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2028237480"/>
+        <c:axId val="-2114351256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7424,7 +7428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092696808"/>
+        <c:crossAx val="-2114354040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7673,11 +7677,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2028269784"/>
-        <c:axId val="-2093435272"/>
+        <c:axId val="-2114299176"/>
+        <c:axId val="-2114296392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2028269784"/>
+        <c:axId val="-2114299176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7687,12 +7691,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093435272"/>
+        <c:crossAx val="-2114296392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093435272"/>
+        <c:axId val="-2114296392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7703,7 +7707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028269784"/>
+        <c:crossAx val="-2114299176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7885,11 +7889,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2028351672"/>
-        <c:axId val="2028386712"/>
+        <c:axId val="-2114267128"/>
+        <c:axId val="-2114264376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2028351672"/>
+        <c:axId val="-2114267128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7899,12 +7903,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028386712"/>
+        <c:crossAx val="-2114264376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2028386712"/>
+        <c:axId val="-2114264376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7915,7 +7919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028351672"/>
+        <c:crossAx val="-2114267128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8097,11 +8101,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2028357384"/>
-        <c:axId val="2028360312"/>
+        <c:axId val="-2114233960"/>
+        <c:axId val="-2114231208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2028357384"/>
+        <c:axId val="-2114233960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8111,12 +8115,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028360312"/>
+        <c:crossAx val="-2114231208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2028360312"/>
+        <c:axId val="-2114231208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8127,7 +8131,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028357384"/>
+        <c:crossAx val="-2114233960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8370,11 +8374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2028261624"/>
-        <c:axId val="2028264328"/>
+        <c:axId val="-2114200424"/>
+        <c:axId val="-2114197640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2028261624"/>
+        <c:axId val="-2114200424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8384,12 +8388,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028264328"/>
+        <c:crossAx val="-2114197640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2028264328"/>
+        <c:axId val="-2114197640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8400,7 +8404,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028261624"/>
+        <c:crossAx val="-2114200424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8643,11 +8647,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2028340552"/>
-        <c:axId val="2028301976"/>
+        <c:axId val="-2114166504"/>
+        <c:axId val="-2114163720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2028340552"/>
+        <c:axId val="-2114166504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8657,12 +8661,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028301976"/>
+        <c:crossAx val="-2114163720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2028301976"/>
+        <c:axId val="-2114163720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8673,7 +8677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028340552"/>
+        <c:crossAx val="-2114166504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8826,11 +8830,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2133214712"/>
-        <c:axId val="2133206648"/>
+        <c:axId val="-2116845128"/>
+        <c:axId val="-2116847880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2133214712"/>
+        <c:axId val="-2116845128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8840,12 +8844,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133206648"/>
+        <c:crossAx val="-2116847880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2133206648"/>
+        <c:axId val="-2116847880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8856,7 +8860,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133214712"/>
+        <c:crossAx val="-2116845128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9105,11 +9109,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093022360"/>
-        <c:axId val="-2093019576"/>
+        <c:axId val="-2114117272"/>
+        <c:axId val="-2114114488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093022360"/>
+        <c:axId val="-2114117272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9119,12 +9123,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093019576"/>
+        <c:crossAx val="-2114114488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093019576"/>
+        <c:axId val="-2114114488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9135,7 +9139,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093022360"/>
+        <c:crossAx val="-2114117272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9317,11 +9321,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092990280"/>
-        <c:axId val="-2092987528"/>
+        <c:axId val="-2077686520"/>
+        <c:axId val="-2077683768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092990280"/>
+        <c:axId val="-2077686520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9331,12 +9335,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092987528"/>
+        <c:crossAx val="-2077683768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092987528"/>
+        <c:axId val="-2077683768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9347,7 +9351,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092990280"/>
+        <c:crossAx val="-2077686520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9529,11 +9533,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116604840"/>
-        <c:axId val="-2095726088"/>
+        <c:axId val="-2077645992"/>
+        <c:axId val="-2077643240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116604840"/>
+        <c:axId val="-2077645992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9543,12 +9547,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095726088"/>
+        <c:crossAx val="-2077643240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2095726088"/>
+        <c:axId val="-2077643240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9559,7 +9563,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116604840"/>
+        <c:crossAx val="-2077645992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9802,11 +9806,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2095447624"/>
-        <c:axId val="-2095444840"/>
+        <c:axId val="-2077592408"/>
+        <c:axId val="-2077589624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2095447624"/>
+        <c:axId val="-2077592408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9816,12 +9820,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095444840"/>
+        <c:crossAx val="-2077589624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2095444840"/>
+        <c:axId val="-2077589624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9832,14 +9836,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095447624"/>
+        <c:crossAx val="-2077592408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10012,11 +10015,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2095415912"/>
-        <c:axId val="-2095413144"/>
+        <c:axId val="-2078575448"/>
+        <c:axId val="-2078603272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2095415912"/>
+        <c:axId val="-2078575448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10026,12 +10029,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095413144"/>
+        <c:crossAx val="-2078603272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2095413144"/>
+        <c:axId val="-2078603272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10042,14 +10045,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095415912"/>
+        <c:crossAx val="-2078575448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10222,11 +10224,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2095382712"/>
-        <c:axId val="-2095379944"/>
+        <c:axId val="-2078527448"/>
+        <c:axId val="-2078524696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2095382712"/>
+        <c:axId val="-2078527448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10236,12 +10238,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095379944"/>
+        <c:crossAx val="-2078524696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2095379944"/>
+        <c:axId val="-2078524696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10252,14 +10254,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095382712"/>
+        <c:crossAx val="-2078527448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10328,7 +10329,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -10472,7 +10472,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -10597,11 +10596,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2095332744"/>
-        <c:axId val="-2095329816"/>
+        <c:axId val="-2078469896"/>
+        <c:axId val="-2078466968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2095332744"/>
+        <c:axId val="-2078469896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10611,12 +10610,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095329816"/>
+        <c:crossAx val="-2078466968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2095329816"/>
+        <c:axId val="-2078466968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10627,14 +10626,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095332744"/>
+        <c:crossAx val="-2078469896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10679,7 +10677,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -10843,11 +10840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2095301160"/>
-        <c:axId val="-2095298376"/>
+        <c:axId val="-2077635880"/>
+        <c:axId val="-2077582616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2095301160"/>
+        <c:axId val="-2077635880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10857,12 +10854,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095298376"/>
+        <c:crossAx val="-2077582616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2095298376"/>
+        <c:axId val="-2077582616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10873,14 +10870,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095301160"/>
+        <c:crossAx val="-2077635880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10925,7 +10921,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -11086,11 +11081,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093005432"/>
-        <c:axId val="-2092979864"/>
+        <c:axId val="-2077540312"/>
+        <c:axId val="-2077537528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093005432"/>
+        <c:axId val="-2077540312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11100,12 +11095,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092979864"/>
+        <c:crossAx val="-2077537528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092979864"/>
+        <c:axId val="-2077537528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11116,14 +11111,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093005432"/>
+        <c:crossAx val="-2077540312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11360,11 +11354,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090030152"/>
-        <c:axId val="-2090027368"/>
+        <c:axId val="-2077486824"/>
+        <c:axId val="-2077484040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2090030152"/>
+        <c:axId val="-2077486824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11374,12 +11368,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090027368"/>
+        <c:crossAx val="-2077484040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2090027368"/>
+        <c:axId val="-2077484040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11390,7 +11384,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090030152"/>
+        <c:crossAx val="-2077486824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11652,11 +11646,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2133140504"/>
-        <c:axId val="2133143432"/>
+        <c:axId val="-2116899976"/>
+        <c:axId val="-2116902872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2133140504"/>
+        <c:axId val="-2116899976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11666,12 +11660,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133143432"/>
+        <c:crossAx val="-2116902872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2133143432"/>
+        <c:axId val="-2116902872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11682,7 +11676,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133140504"/>
+        <c:crossAx val="-2116899976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11861,11 +11855,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090000872"/>
-        <c:axId val="-2089998120"/>
+        <c:axId val="-2077454296"/>
+        <c:axId val="-2077451544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2090000872"/>
+        <c:axId val="-2077454296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11875,12 +11869,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089998120"/>
+        <c:crossAx val="-2077451544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089998120"/>
+        <c:axId val="-2077451544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11891,7 +11885,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090000872"/>
+        <c:crossAx val="-2077454296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12071,11 +12065,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089016680"/>
-        <c:axId val="-2088978424"/>
+        <c:axId val="-2077421272"/>
+        <c:axId val="-2077418520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089016680"/>
+        <c:axId val="-2077421272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12085,12 +12079,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088978424"/>
+        <c:crossAx val="-2077418520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2088978424"/>
+        <c:axId val="-2077418520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12101,7 +12095,701 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089016680"/>
+        <c:crossAx val="-2077421272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels EP2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels EP2'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels EP2'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>144.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>175.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>212.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>238.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>265.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>272.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels EP2'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rspeed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.286665786441329"/>
+                  <c:y val="0.0219323609139022"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels EP2'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels EP2'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>211.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>241.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>262.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>267.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2079359448"/>
+        <c:axId val="-2079356664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2079359448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2079356664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2079356664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2079359448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels EP2'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0579260404949381"/>
+                  <c:y val="0.028316961194183"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels EP2'!$B$3:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>144.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>175.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>212.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>238.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>265.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels EP2'!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2061004552"/>
+        <c:axId val="2061007480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2061004552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2061007480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2061007480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2061004552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RPower</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.439526023342827"/>
+          <c:y val="0.0328467153284671"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Wheels EP2'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.123849409448819"/>
+                  <c:y val="0.0421526584421247"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.00000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wheels EP2'!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>211.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>241.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>262.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wheels EP2'!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2061036936"/>
+        <c:axId val="2061039864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2061036936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2061039864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2061039864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2061036936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12261,11 +12949,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2132915960"/>
-        <c:axId val="2132892920"/>
+        <c:axId val="-2116930680"/>
+        <c:axId val="-2116933432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2132915960"/>
+        <c:axId val="-2116930680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12275,12 +12963,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132892920"/>
+        <c:crossAx val="-2116933432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2132892920"/>
+        <c:axId val="-2116933432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12291,7 +12979,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132915960"/>
+        <c:crossAx val="-2116930680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12444,11 +13132,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2132840200"/>
-        <c:axId val="2132843096"/>
+        <c:axId val="-2116963176"/>
+        <c:axId val="-2116965928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2132840200"/>
+        <c:axId val="-2116963176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12458,12 +13146,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132843096"/>
+        <c:crossAx val="-2116965928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2132843096"/>
+        <c:axId val="-2116965928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12474,7 +13162,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132840200"/>
+        <c:crossAx val="-2116963176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12699,11 +13387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093740264"/>
-        <c:axId val="-2093737336"/>
+        <c:axId val="-2121027176"/>
+        <c:axId val="-2121030072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093740264"/>
+        <c:axId val="-2121027176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12713,12 +13401,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093737336"/>
+        <c:crossAx val="-2121030072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093737336"/>
+        <c:axId val="-2121030072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12729,7 +13417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093740264"/>
+        <c:crossAx val="-2121027176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12870,11 +13558,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093709624"/>
-        <c:axId val="-2093706840"/>
+        <c:axId val="-2121069608"/>
+        <c:axId val="-2121072360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093709624"/>
+        <c:axId val="-2121069608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12884,12 +13572,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093706840"/>
+        <c:crossAx val="-2121072360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093706840"/>
+        <c:axId val="-2121072360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12900,7 +13588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093709624"/>
+        <c:crossAx val="-2121069608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13556,6 +14244,107 @@
 </file>
 
 <file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -16259,7 +17048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -16388,6 +17177,159 @@
     <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0.1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>70</v>
+      </c>
+      <c r="C4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>104</v>
+      </c>
+      <c r="C5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>144</v>
+      </c>
+      <c r="C6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>175</v>
+      </c>
+      <c r="C7">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>212</v>
+      </c>
+      <c r="C8">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>238</v>
+      </c>
+      <c r="C9">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>265</v>
+      </c>
+      <c r="C10">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>272</v>
+      </c>
+      <c r="C11">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>